<commit_message>
Export construction list and update InputJSONData.xlsx for HVAC tab per Sumit
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwell\P+W SPEED Dropbox\Research\SPEED\WebGUI\Specifications\DataIntegrity\SPEEDInputJSON_Dan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E87B498-93D7-4637-BF38-151A1C22676F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABB0144-C838-4F94-A652-C685387A1F1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="229">
   <si>
     <t>Primary_Building_Type</t>
   </si>
@@ -301,9 +292,6 @@
     <t>Space_Type</t>
   </si>
   <si>
-    <t>HVAC_Type</t>
-  </si>
-  <si>
     <t>Hospital-Lab</t>
   </si>
   <si>
@@ -730,7 +718,7 @@
     <t>Analysis_Type_2_3</t>
   </si>
   <si>
-    <t>HVAC</t>
+    <t>HVAC_TYPE</t>
   </si>
 </sst>
 </file>
@@ -784,7 +772,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -853,6 +841,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -862,7 +861,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -919,13 +918,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -946,7 +948,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1274,19 +1276,19 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B1" s="23"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1302,91 +1304,91 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -1408,14 +1410,14 @@
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.86328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.1328125" style="9"/>
-    <col min="8" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="1" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.109375" style="9"/>
+    <col min="8" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1431,12 +1433,12 @@
       <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>150</v>
       </c>
@@ -1482,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1493,7 +1495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1504,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1515,7 +1517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1526,7 +1528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1537,7 +1539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1548,7 +1550,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1559,7 +1561,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1570,7 +1572,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1581,7 +1583,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1592,7 +1594,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1603,7 +1605,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1614,7 +1616,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1625,7 +1627,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1636,7 +1638,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1647,7 +1649,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1658,7 +1660,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1669,7 +1671,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1680,7 +1682,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1691,7 +1693,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1702,7 +1704,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1713,7 +1715,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1724,7 +1726,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1735,7 +1737,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1746,7 +1748,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1757,7 +1759,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1768,7 +1770,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1779,7 +1781,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1790,7 +1792,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1801,7 +1803,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1812,7 +1814,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1823,7 +1825,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1834,7 +1836,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1845,7 +1847,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1856,7 +1858,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1867,7 +1869,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1878,7 +1880,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1889,7 +1891,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1900,7 +1902,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1911,7 +1913,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1922,7 +1924,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1933,7 +1935,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1944,7 +1946,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1955,7 +1957,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1966,7 +1968,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1977,7 +1979,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1988,7 +1990,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1999,7 +2001,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2010,7 +2012,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2021,7 +2023,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -2032,7 +2034,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2043,7 +2045,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -2054,7 +2056,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2065,7 +2067,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -2076,7 +2078,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2087,7 +2089,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2098,7 +2100,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2109,7 +2111,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2120,7 +2122,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2131,7 +2133,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2142,7 +2144,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2153,7 +2155,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2164,7 +2166,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2175,7 +2177,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2186,7 +2188,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2197,7 +2199,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2208,7 +2210,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2219,7 +2221,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2230,7 +2232,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -2241,7 +2243,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2252,7 +2254,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2276,148 +2278,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E11A7-4D06-4105-860E-F3792C5BE0ED}">
   <dimension ref="A1:BN143"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AU3" sqref="AU3:AW17"/>
+    <sheetView topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.06640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.73046875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.1328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="18.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="10.265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="18.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="10.265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="18.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="10.265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="18.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="10.265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="18.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="10.265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="18.59765625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.73046875" style="9" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.46484375" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="14" style="9" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18.9296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.9296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.9296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7.46484375" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.9296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="7.46484375" style="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.9296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.46484375" style="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.1328125" style="9"/>
+    <col min="63" max="63" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="67" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22"/>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22" t="s">
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="23" t="s">
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23"/>
-      <c r="BG1" s="23"/>
-      <c r="BH1" s="23"/>
-      <c r="BI1" s="23"/>
-      <c r="BJ1" s="23"/>
-      <c r="BK1" s="23"/>
-      <c r="BL1" s="23"/>
-      <c r="BM1" s="23"/>
-      <c r="BN1" s="23"/>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+    </row>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2433,14 +2435,14 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="I2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="I2" s="23"/>
       <c r="J2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2450,110 +2452,110 @@
       <c r="L2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22" t="s">
+      <c r="N2" s="23"/>
+      <c r="O2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="22"/>
+      <c r="P2" s="23"/>
       <c r="Q2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="R2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22" t="s">
+      <c r="S2" s="23"/>
+      <c r="T2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="22"/>
+      <c r="U2" s="23"/>
       <c r="V2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="22" t="s">
+      <c r="W2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22" t="s">
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="22"/>
+      <c r="Z2" s="23"/>
       <c r="AA2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AB2" s="22" t="s">
+      <c r="AB2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22" t="s">
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" s="22"/>
+      <c r="AE2" s="23"/>
       <c r="AF2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="22" t="s">
+      <c r="AG2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="22" t="s">
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AJ2" s="22"/>
+      <c r="AJ2" s="23"/>
       <c r="AK2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AL2" s="22" t="s">
+      <c r="AL2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22" t="s">
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AO2" s="22"/>
+      <c r="AO2" s="23"/>
       <c r="AP2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AQ2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AR2" s="22" t="s">
+      <c r="AR2" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="22"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="22" t="s">
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="23"/>
+      <c r="AU2" s="23"/>
+      <c r="AV2" s="23"/>
+      <c r="AW2" s="23"/>
+      <c r="AX2" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AY2" s="22"/>
-      <c r="AZ2" s="22"/>
-      <c r="BA2" s="22"/>
-      <c r="BB2" s="22"/>
-      <c r="BC2" s="22"/>
-      <c r="BD2" s="22"/>
-      <c r="BE2" s="22" t="s">
+      <c r="AY2" s="23"/>
+      <c r="AZ2" s="23"/>
+      <c r="BA2" s="23"/>
+      <c r="BB2" s="23"/>
+      <c r="BC2" s="23"/>
+      <c r="BD2" s="23"/>
+      <c r="BE2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="BF2" s="22"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22" t="s">
+      <c r="BF2" s="23"/>
+      <c r="BG2" s="23"/>
+      <c r="BH2" s="23"/>
+      <c r="BI2" s="23"/>
+      <c r="BJ2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
+      <c r="BK2" s="23"/>
+      <c r="BL2" s="23"/>
+      <c r="BM2" s="23"/>
       <c r="BN2" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>200000</v>
       </c>
@@ -2747,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2937,7 +2939,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3">
@@ -3095,7 +3097,7 @@
       </c>
       <c r="BN5" s="10"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -3203,7 +3205,7 @@
       </c>
       <c r="BN6" s="10"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -3309,7 +3311,7 @@
       </c>
       <c r="BN7" s="10"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -3415,7 +3417,7 @@
       </c>
       <c r="BN8" s="10"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3">
@@ -3519,7 +3521,7 @@
       </c>
       <c r="BN9" s="10"/>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -3617,7 +3619,7 @@
       <c r="BM10" s="3"/>
       <c r="BN10" s="3"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -3715,7 +3717,7 @@
       <c r="BM11" s="3"/>
       <c r="BN11" s="3"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3">
@@ -3813,7 +3815,7 @@
       <c r="BM12" s="3"/>
       <c r="BN12" s="3"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3911,7 +3913,7 @@
       <c r="BM13" s="3"/>
       <c r="BN13" s="3"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3">
@@ -4009,7 +4011,7 @@
       <c r="BM14" s="3"/>
       <c r="BN14" s="3"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -4107,7 +4109,7 @@
       <c r="BM15" s="3"/>
       <c r="BN15" s="3"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -4205,7 +4207,7 @@
       <c r="BM16" s="3"/>
       <c r="BN16" s="3"/>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -4279,7 +4281,7 @@
       <c r="BM17" s="3"/>
       <c r="BN17" s="3"/>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -4353,7 +4355,7 @@
       <c r="BM18" s="3"/>
       <c r="BN18" s="3"/>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -4427,7 +4429,7 @@
       <c r="BM19" s="3"/>
       <c r="BN19" s="3"/>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -4501,7 +4503,7 @@
       <c r="BM20" s="3"/>
       <c r="BN20" s="3"/>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -4575,7 +4577,7 @@
       <c r="BM21" s="3"/>
       <c r="BN21" s="3"/>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -4649,7 +4651,7 @@
       <c r="BM22" s="3"/>
       <c r="BN22" s="3"/>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -4723,7 +4725,7 @@
       <c r="BM23" s="3"/>
       <c r="BN23" s="3"/>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -4797,7 +4799,7 @@
       <c r="BM24" s="3"/>
       <c r="BN24" s="3"/>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3">
@@ -4871,7 +4873,7 @@
       <c r="BM25" s="3"/>
       <c r="BN25" s="3"/>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3">
@@ -4945,7 +4947,7 @@
       <c r="BM26" s="3"/>
       <c r="BN26" s="3"/>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
@@ -5019,7 +5021,7 @@
       <c r="BM27" s="3"/>
       <c r="BN27" s="3"/>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
@@ -5093,7 +5095,7 @@
       <c r="BM28" s="3"/>
       <c r="BN28" s="3"/>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
@@ -5167,7 +5169,7 @@
       <c r="BM29" s="3"/>
       <c r="BN29" s="3"/>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
@@ -5241,7 +5243,7 @@
       <c r="BM30" s="3"/>
       <c r="BN30" s="3"/>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
@@ -5315,7 +5317,7 @@
       <c r="BM31" s="3"/>
       <c r="BN31" s="3"/>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
@@ -5389,7 +5391,7 @@
       <c r="BM32" s="3"/>
       <c r="BN32" s="3"/>
     </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3">
@@ -5463,7 +5465,7 @@
       <c r="BM33" s="3"/>
       <c r="BN33" s="3"/>
     </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
@@ -5537,7 +5539,7 @@
       <c r="BM34" s="3"/>
       <c r="BN34" s="3"/>
     </row>
-    <row r="35" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
@@ -5611,7 +5613,7 @@
       <c r="BM35" s="3"/>
       <c r="BN35" s="3"/>
     </row>
-    <row r="36" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
@@ -5683,7 +5685,7 @@
       <c r="BM36" s="3"/>
       <c r="BN36" s="3"/>
     </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3">
@@ -5755,7 +5757,7 @@
       <c r="BM37" s="3"/>
       <c r="BN37" s="3"/>
     </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3">
@@ -5827,7 +5829,7 @@
       <c r="BM38" s="3"/>
       <c r="BN38" s="3"/>
     </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3">
@@ -5899,7 +5901,7 @@
       <c r="BM39" s="3"/>
       <c r="BN39" s="3"/>
     </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3">
@@ -5971,7 +5973,7 @@
       <c r="BM40" s="3"/>
       <c r="BN40" s="3"/>
     </row>
-    <row r="41" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3">
@@ -6043,7 +6045,7 @@
       <c r="BM41" s="3"/>
       <c r="BN41" s="3"/>
     </row>
-    <row r="42" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3">
@@ -6115,7 +6117,7 @@
       <c r="BM42" s="3"/>
       <c r="BN42" s="3"/>
     </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3">
@@ -6187,7 +6189,7 @@
       <c r="BM43" s="3"/>
       <c r="BN43" s="3"/>
     </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3">
@@ -6259,7 +6261,7 @@
       <c r="BM44" s="3"/>
       <c r="BN44" s="3"/>
     </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3">
@@ -6331,7 +6333,7 @@
       <c r="BM45" s="3"/>
       <c r="BN45" s="3"/>
     </row>
-    <row r="46" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
@@ -6403,7 +6405,7 @@
       <c r="BM46" s="3"/>
       <c r="BN46" s="3"/>
     </row>
-    <row r="47" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3">
@@ -6475,7 +6477,7 @@
       <c r="BM47" s="3"/>
       <c r="BN47" s="3"/>
     </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3">
@@ -6547,7 +6549,7 @@
       <c r="BM48" s="3"/>
       <c r="BN48" s="3"/>
     </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3">
@@ -6619,7 +6621,7 @@
       <c r="BM49" s="3"/>
       <c r="BN49" s="3"/>
     </row>
-    <row r="50" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3">
@@ -6691,7 +6693,7 @@
       <c r="BM50" s="3"/>
       <c r="BN50" s="3"/>
     </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3">
@@ -6763,7 +6765,7 @@
       <c r="BM51" s="3"/>
       <c r="BN51" s="3"/>
     </row>
-    <row r="52" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3">
@@ -6835,7 +6837,7 @@
       <c r="BM52" s="3"/>
       <c r="BN52" s="3"/>
     </row>
-    <row r="53" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6905,7 +6907,7 @@
       <c r="BM53" s="3"/>
       <c r="BN53" s="3"/>
     </row>
-    <row r="54" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6975,7 +6977,7 @@
       <c r="BM54" s="3"/>
       <c r="BN54" s="3"/>
     </row>
-    <row r="55" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -7045,7 +7047,7 @@
       <c r="BM55" s="3"/>
       <c r="BN55" s="3"/>
     </row>
-    <row r="56" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -7115,7 +7117,7 @@
       <c r="BM56" s="3"/>
       <c r="BN56" s="3"/>
     </row>
-    <row r="57" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -7185,7 +7187,7 @@
       <c r="BM57" s="3"/>
       <c r="BN57" s="3"/>
     </row>
-    <row r="58" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -7255,7 +7257,7 @@
       <c r="BM58" s="3"/>
       <c r="BN58" s="3"/>
     </row>
-    <row r="59" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -7325,7 +7327,7 @@
       <c r="BM59" s="3"/>
       <c r="BN59" s="3"/>
     </row>
-    <row r="60" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -7395,7 +7397,7 @@
       <c r="BM60" s="3"/>
       <c r="BN60" s="3"/>
     </row>
-    <row r="61" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -7465,7 +7467,7 @@
       <c r="BM61" s="3"/>
       <c r="BN61" s="3"/>
     </row>
-    <row r="62" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -7535,7 +7537,7 @@
       <c r="BM62" s="3"/>
       <c r="BN62" s="3"/>
     </row>
-    <row r="63" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -7605,7 +7607,7 @@
       <c r="BM63" s="3"/>
       <c r="BN63" s="3"/>
     </row>
-    <row r="64" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -7675,7 +7677,7 @@
       <c r="BM64" s="3"/>
       <c r="BN64" s="3"/>
     </row>
-    <row r="65" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -7745,7 +7747,7 @@
       <c r="BM65" s="3"/>
       <c r="BN65" s="3"/>
     </row>
-    <row r="66" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -7815,7 +7817,7 @@
       <c r="BM66" s="3"/>
       <c r="BN66" s="3"/>
     </row>
-    <row r="67" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -7885,7 +7887,7 @@
       <c r="BM67" s="3"/>
       <c r="BN67" s="3"/>
     </row>
-    <row r="68" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -7955,7 +7957,7 @@
       <c r="BM68" s="3"/>
       <c r="BN68" s="3"/>
     </row>
-    <row r="69" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -8025,7 +8027,7 @@
       <c r="BM69" s="3"/>
       <c r="BN69" s="3"/>
     </row>
-    <row r="70" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -8095,7 +8097,7 @@
       <c r="BM70" s="3"/>
       <c r="BN70" s="3"/>
     </row>
-    <row r="71" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -8165,7 +8167,7 @@
       <c r="BM71" s="3"/>
       <c r="BN71" s="3"/>
     </row>
-    <row r="72" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -8235,7 +8237,7 @@
       <c r="BM72" s="3"/>
       <c r="BN72" s="3"/>
     </row>
-    <row r="73" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -8305,7 +8307,7 @@
       <c r="BM73" s="3"/>
       <c r="BN73" s="3"/>
     </row>
-    <row r="74" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -8375,11 +8377,11 @@
       <c r="BM74" s="3"/>
       <c r="BN74" s="3"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -8394,26 +8396,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BH3:BI3"/>
-    <mergeCell ref="BL3:BM3"/>
-    <mergeCell ref="AR2:AW2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BE2:BI2"/>
-    <mergeCell ref="BJ2:BM2"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:BN1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:AO1"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="AL2:AM2"/>
     <mergeCell ref="F2:G2"/>
@@ -8422,6 +8404,26 @@
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:BN1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:AO1"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BH3:BI3"/>
+    <mergeCell ref="BL3:BM3"/>
+    <mergeCell ref="AR2:AW2"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="BE2:BI2"/>
+    <mergeCell ref="BJ2:BM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AD2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8436,43 +8438,43 @@
       <selection activeCell="J23" sqref="A23:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" style="9" customWidth="1"/>
-    <col min="5" max="6" width="9.1328125" style="9"/>
-    <col min="7" max="7" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="9" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="9"/>
+    <col min="7" max="7" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.59765625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="7"/>
+    <col min="11" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8504,7 +8506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -8544,7 +8546,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>5</v>
@@ -8567,7 +8569,7 @@
       </c>
       <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>10</v>
@@ -8589,7 +8591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>15</v>
@@ -8611,7 +8613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>20</v>
@@ -8633,7 +8635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>25</v>
@@ -8655,7 +8657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>30</v>
@@ -8677,7 +8679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>35</v>
@@ -8699,7 +8701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>40</v>
@@ -8721,7 +8723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>45</v>
@@ -8743,7 +8745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>50</v>
@@ -8765,7 +8767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>55</v>
@@ -8788,7 +8790,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>60</v>
@@ -8815,7 +8817,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>65</v>
@@ -8837,7 +8839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>70</v>
@@ -8859,7 +8861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>75</v>
@@ -8881,7 +8883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>80</v>
@@ -8914,7 +8916,7 @@
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>85</v>
@@ -8934,7 +8936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>90</v>
@@ -8954,7 +8956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>95</v>
@@ -8974,7 +8976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8990,55 +8992,55 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" s="14"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="14"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="14"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="14"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="14"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="14"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="14"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="14"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="14"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="14"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="14"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="14"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="14"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="14"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="14"/>
     </row>
   </sheetData>
@@ -9062,20 +9064,20 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="1" width="12.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="28"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -9083,756 +9085,756 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="18" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="16"/>
       <c r="B103" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="16"/>
       <c r="B104" s="18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
       <c r="B105" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="16"/>
       <c r="B106" s="18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="16"/>
       <c r="B107" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="16"/>
       <c r="B108" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
       <c r="B109" s="18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="16"/>
       <c r="B110" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="16"/>
       <c r="B111" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="16"/>
       <c r="B113" s="18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="16"/>
       <c r="B114" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="16"/>
       <c r="B115" s="18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="16"/>
       <c r="B116" s="18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="16"/>
       <c r="B117" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="16"/>
       <c r="B118" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="16"/>
       <c r="B119" s="18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="16"/>
       <c r="B120" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="16"/>
       <c r="B121" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="16"/>
       <c r="B123" s="18" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="16"/>
       <c r="B124" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="16"/>
       <c r="B125" s="18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="16"/>
       <c r="B126" s="18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="16"/>
       <c r="B127" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -9852,61 +9854,61 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="1" width="43.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="29" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="F2" s="30"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="E3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="F3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="15" t="s">
-        <v>99</v>
-      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
         <v>92</v>
       </c>
@@ -9923,7 +9925,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
         <v>93</v>
@@ -9937,7 +9939,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
         <v>94</v>
@@ -9951,7 +9953,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
         <v>95</v>
@@ -9965,7 +9967,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
         <v>96</v>
@@ -9979,7 +9981,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
         <v>97</v>
@@ -9993,7 +9995,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="15" t="s">
         <v>98</v>
@@ -10003,7 +10005,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
         <v>99</v>
@@ -10013,7 +10015,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
         <v>100</v>
@@ -10023,22 +10025,14 @@
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="1"/>
-      <c r="B13" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
+  <mergeCells count="3">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -10053,21 +10047,21 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.1328125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="1" width="19.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="22"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="23"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -10075,18 +10069,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -10105,20 +10099,20 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" style="9"/>
-    <col min="3" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="1" width="11.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="9"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="22"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="23"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -10126,7 +10120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>50</v>
       </c>
@@ -10134,115 +10128,115 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
Updated InputJSONData.xlsx spreadsheet to match expected JSON structure
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABB0144-C838-4F94-A652-C685387A1F1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E46367-53EE-47E4-91B6-CD6FDF92BA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="2" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -861,7 +861,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -924,6 +924,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -936,19 +951,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1283,10 +1289,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1433,10 +1439,10 @@
       <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2278,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E11A7-4D06-4105-860E-F3792C5BE0ED}">
   <dimension ref="A1:BN143"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2339,85 +2345,83 @@
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="23" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="23"/>
-      <c r="AR1" s="25" t="s">
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="25"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="25"/>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="25"/>
-      <c r="AZ1" s="25"/>
-      <c r="BA1" s="25"/>
-      <c r="BB1" s="25"/>
-      <c r="BC1" s="25"/>
-      <c r="BD1" s="25"/>
-      <c r="BE1" s="25"/>
-      <c r="BF1" s="25"/>
-      <c r="BG1" s="25"/>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+      <c r="BN1" s="30"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2435,122 +2439,88 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="25"/>
       <c r="J2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="23"/>
-      <c r="V2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO2" s="23"/>
+      <c r="L2" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
       <c r="AP2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AQ2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AR2" s="23" t="s">
+      <c r="AR2" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="23" t="s">
+      <c r="AS2" s="25"/>
+      <c r="AT2" s="25"/>
+      <c r="AU2" s="25"/>
+      <c r="AV2" s="25"/>
+      <c r="AW2" s="25"/>
+      <c r="AX2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AY2" s="23"/>
-      <c r="AZ2" s="23"/>
-      <c r="BA2" s="23"/>
-      <c r="BB2" s="23"/>
-      <c r="BC2" s="23"/>
-      <c r="BD2" s="23"/>
-      <c r="BE2" s="23" t="s">
+      <c r="AY2" s="25"/>
+      <c r="AZ2" s="25"/>
+      <c r="BA2" s="25"/>
+      <c r="BB2" s="25"/>
+      <c r="BC2" s="25"/>
+      <c r="BD2" s="25"/>
+      <c r="BE2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="BF2" s="23"/>
-      <c r="BG2" s="23"/>
-      <c r="BH2" s="23"/>
-      <c r="BI2" s="23"/>
-      <c r="BJ2" s="23" t="s">
+      <c r="BF2" s="25"/>
+      <c r="BG2" s="25"/>
+      <c r="BH2" s="25"/>
+      <c r="BI2" s="25"/>
+      <c r="BJ2" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="BK2" s="23"/>
-      <c r="BL2" s="23"/>
-      <c r="BM2" s="23"/>
+      <c r="BK2" s="25"/>
+      <c r="BL2" s="25"/>
+      <c r="BM2" s="25"/>
       <c r="BN2" s="5" t="s">
         <v>47</v>
       </c>
@@ -2589,96 +2559,48 @@
       <c r="K3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="L3" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="28"/>
+      <c r="AK3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="27"/>
+      <c r="AO3" s="28"/>
       <c r="AP3" s="3">
         <v>0</v>
       </c>
@@ -2718,10 +2640,10 @@
       <c r="BB3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BC3" s="24" t="s">
+      <c r="BC3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="BD3" s="24"/>
+      <c r="BD3" s="29"/>
       <c r="BE3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2731,20 +2653,20 @@
       <c r="BG3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BH3" s="24" t="s">
+      <c r="BH3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="BI3" s="24"/>
+      <c r="BI3" s="29"/>
       <c r="BJ3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BK3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BL3" s="24" t="s">
+      <c r="BL3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="BM3" s="24"/>
+      <c r="BM3" s="29"/>
       <c r="BN3" s="10" t="s">
         <v>1</v>
       </c>
@@ -2775,96 +2697,60 @@
       <c r="K4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="3">
-        <v>5</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>7</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="V4" s="3">
-        <v>13</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>9</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF4" s="3">
-        <v>13</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK4" s="3">
-        <v>9</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="L4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" s="27"/>
+      <c r="AI4" s="27"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AL4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="27"/>
+      <c r="AO4" s="28"/>
       <c r="AP4" s="3"/>
       <c r="AQ4" s="3">
         <v>5</v>
@@ -2959,72 +2845,84 @@
       <c r="K5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="3">
+        <v>5</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="N5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="3">
+        <v>7</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="S5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="T5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="25"/>
+      <c r="V5" s="3">
+        <v>13</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="X5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="Y5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="3">
+        <v>9</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AC5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="AD5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="3">
+        <v>13</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AH5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="AI5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ5" s="25"/>
+      <c r="AK5" s="3">
+        <v>9</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AM5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO5" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO5" s="25"/>
       <c r="AP5" s="3"/>
       <c r="AQ5" s="3">
         <v>10</v>
@@ -3118,58 +3016,82 @@
         <v>42</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="O6" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="T6" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
+      <c r="W6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="Y6" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
+      <c r="AB6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AD6" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
+      <c r="AG6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AI6" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
+      <c r="AL6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AN6" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="AO6" s="3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="AP6" s="3"/>
       <c r="AQ6" s="3">
@@ -3225,57 +3147,69 @@
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="O7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="T7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
+      <c r="X7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="Y7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
+      <c r="AC7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="AD7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
+      <c r="AH7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="AI7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
+      <c r="AM7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="AN7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AO7" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AP7" s="3"/>
       <c r="AQ7" s="3">
@@ -3333,55 +3267,55 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA8" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF8" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK8" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
       <c r="AM8" s="3"/>
       <c r="AN8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AO8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AP8" s="3"/>
       <c r="AQ8" s="3">
@@ -3433,8 +3367,8 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3" t="s">
         <v>71</v>
@@ -3442,8 +3376,8 @@
       <c r="P9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3" t="s">
         <v>71</v>
@@ -3451,8 +3385,8 @@
       <c r="U9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3" t="s">
         <v>71</v>
@@ -3460,8 +3394,8 @@
       <c r="Z9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="5"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3" t="s">
         <v>71</v>
@@ -3469,8 +3403,8 @@
       <c r="AE9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="5"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="3" t="s">
         <v>71</v>
@@ -3478,8 +3412,8 @@
       <c r="AJ9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="5"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="3"/>
       <c r="AM9" s="3"/>
       <c r="AN9" s="3" t="s">
         <v>71</v>
@@ -3537,7 +3471,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="5"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3" t="s">
@@ -3546,7 +3480,7 @@
       <c r="P10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Q10" s="3"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3" t="s">
@@ -3555,7 +3489,7 @@
       <c r="U10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="V10" s="3"/>
+      <c r="V10" s="5"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3" t="s">
@@ -3636,58 +3570,58 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="R11" s="5"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
+      <c r="W11" s="5"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
+      <c r="AB11" s="5"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
+      <c r="AG11" s="5"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="AK11" s="3"/>
-      <c r="AL11" s="3"/>
+      <c r="AL11" s="5"/>
       <c r="AM11" s="3"/>
       <c r="AN11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="AO11" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="AP11" s="3"/>
       <c r="AQ11" s="3">
@@ -3733,8 +3667,8 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3" t="s">
         <v>71</v>
@@ -3742,8 +3676,8 @@
       <c r="P12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3" t="s">
         <v>71</v>
@@ -3751,8 +3685,8 @@
       <c r="U12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3" t="s">
         <v>71</v>
@@ -3761,7 +3695,7 @@
         <v>71</v>
       </c>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="5"/>
+      <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3" t="s">
         <v>71</v>
@@ -3770,7 +3704,7 @@
         <v>71</v>
       </c>
       <c r="AF12" s="3"/>
-      <c r="AG12" s="5"/>
+      <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3" t="s">
         <v>71</v>
@@ -3779,7 +3713,7 @@
         <v>71</v>
       </c>
       <c r="AK12" s="3"/>
-      <c r="AL12" s="5"/>
+      <c r="AL12" s="3"/>
       <c r="AM12" s="3"/>
       <c r="AN12" s="3" t="s">
         <v>71</v>
@@ -3831,59 +3765,59 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="5"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q13" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="Q13" s="5"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="V13" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="V13" s="5"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AE13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
       <c r="AM13" s="3"/>
       <c r="AN13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AO13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AP13" s="3"/>
       <c r="AQ13" s="3">
@@ -3929,59 +3863,59 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="L14" s="3"/>
       <c r="M14" s="5"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q14" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="Q14" s="3"/>
       <c r="R14" s="5"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="V14" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="V14" s="3"/>
       <c r="W14" s="5"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AA14" s="3"/>
       <c r="AB14" s="5"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AE14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AF14" s="3"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AJ14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AK14" s="3"/>
       <c r="AL14" s="5"/>
       <c r="AM14" s="3"/>
       <c r="AN14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AO14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AP14" s="5"/>
       <c r="AQ14" s="3">
@@ -4027,7 +3961,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="5"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3" t="s">
@@ -4036,7 +3970,7 @@
       <c r="P15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q15" s="3"/>
+      <c r="Q15" s="5"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3" t="s">
@@ -4045,7 +3979,7 @@
       <c r="U15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="V15" s="3"/>
+      <c r="V15" s="5"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="3" t="s">
@@ -4126,7 +4060,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3" t="s">
         <v>78</v>
@@ -4135,7 +4069,7 @@
         <v>78</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
+      <c r="R16" s="5"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3" t="s">
         <v>78</v>
@@ -4144,7 +4078,7 @@
         <v>78</v>
       </c>
       <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="W16" s="5"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3" t="s">
         <v>78</v>
@@ -4153,7 +4087,7 @@
         <v>78</v>
       </c>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
+      <c r="AB16" s="5"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3" t="s">
         <v>78</v>
@@ -4162,7 +4096,7 @@
         <v>78</v>
       </c>
       <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
+      <c r="AG16" s="5"/>
       <c r="AH16" s="3"/>
       <c r="AI16" s="3" t="s">
         <v>78</v>
@@ -4171,7 +4105,7 @@
         <v>78</v>
       </c>
       <c r="AK16" s="3"/>
-      <c r="AL16" s="3"/>
+      <c r="AL16" s="5"/>
       <c r="AM16" s="3"/>
       <c r="AN16" s="3" t="s">
         <v>78</v>
@@ -4226,33 +4160,57 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="O17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
+      <c r="T17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
+      <c r="Y17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
+      <c r="AD17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
-      <c r="AJ17" s="3"/>
+      <c r="AI17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AK17" s="3"/>
       <c r="AL17" s="3"/>
       <c r="AM17" s="3"/>
-      <c r="AN17" s="3"/>
-      <c r="AO17" s="3"/>
+      <c r="AN17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AP17" s="3"/>
       <c r="AQ17" s="3">
         <v>70</v>
@@ -4300,33 +4258,57 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="O18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
+      <c r="T18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
+      <c r="Y18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
+      <c r="AD18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="3"/>
+      <c r="AI18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AK18" s="3"/>
       <c r="AL18" s="3"/>
       <c r="AM18" s="3"/>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="3"/>
+      <c r="AN18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AP18" s="3"/>
       <c r="AQ18" s="3">
         <v>75</v>
@@ -4374,33 +4356,57 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="O19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
+      <c r="T19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
+      <c r="Y19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
+      <c r="AD19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
+      <c r="AI19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AK19" s="3"/>
       <c r="AL19" s="3"/>
       <c r="AM19" s="3"/>
-      <c r="AN19" s="3"/>
-      <c r="AO19" s="3"/>
+      <c r="AN19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AP19" s="3"/>
       <c r="AQ19" s="3">
         <v>80</v>
@@ -8395,35 +8401,41 @@
       <c r="M143" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="AL2:AM2"/>
+  <mergeCells count="34">
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="M4:P4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L2:AO2"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="AG4:AJ4"/>
+    <mergeCell ref="AB4:AE4"/>
+    <mergeCell ref="W4:Z4"/>
     <mergeCell ref="AP1:AQ1"/>
     <mergeCell ref="AR1:BN1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:AO1"/>
-    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="J1:AO1"/>
     <mergeCell ref="BH3:BI3"/>
     <mergeCell ref="BL3:BM3"/>
     <mergeCell ref="AR2:AW2"/>
     <mergeCell ref="AX2:BD2"/>
     <mergeCell ref="BE2:BI2"/>
     <mergeCell ref="BJ2:BM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AD5:AE5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8453,26 +8465,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="27" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="26"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9072,10 +9084,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -9850,7 +9862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84235012-AF5A-4BF0-8557-E62F3FAF9D19}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -9862,14 +9874,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -9878,14 +9890,14 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="31"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -10056,10 +10068,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -10107,10 +10119,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
Updates to InputJSONData.xlsx from Sumit
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E46367-53EE-47E4-91B6-CD6FDF92BA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52745A2-05F0-4A54-AF68-A1CAA300BAD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="2" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="6204" tabRatio="868" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="231">
   <si>
     <t>Primary_Building_Type</t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>HVAC_TYPE</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -861,7 +867,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -930,6 +936,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -939,10 +948,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1276,113 +1285,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB7C557-225C-4221-ACEB-8B371FDF63E0}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="26"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
@@ -1401,8 +1440,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1439,10 +1479,10 @@
       <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="25"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2282,124 +2322,123 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E11A7-4D06-4105-860E-F3792C5BE0ED}">
-  <dimension ref="A1:BN143"/>
+  <dimension ref="A1:BM143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:P4"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="7.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.109375" style="9"/>
+    <col min="8" max="8" width="17.109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="25" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="30" t="s">
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="30" t="s">
         <v>33</v>
       </c>
+      <c r="AR1" s="30"/>
       <c r="AS1" s="30"/>
       <c r="AT1" s="30"/>
       <c r="AU1" s="30"/>
@@ -2421,9 +2460,8 @@
       <c r="BK1" s="30"/>
       <c r="BL1" s="30"/>
       <c r="BM1" s="30"/>
-      <c r="BN1" s="30"/>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2439,93 +2477,92 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="25"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="I2" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="J2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="AP2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR2" s="25" t="s">
+      <c r="AQ2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" s="25"/>
-      <c r="AT2" s="25"/>
-      <c r="AU2" s="25"/>
-      <c r="AV2" s="25"/>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="25" t="s">
+      <c r="AR2" s="26"/>
+      <c r="AS2" s="26"/>
+      <c r="AT2" s="26"/>
+      <c r="AU2" s="26"/>
+      <c r="AV2" s="26"/>
+      <c r="AW2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AY2" s="25"/>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="25"/>
-      <c r="BE2" s="25" t="s">
+      <c r="AX2" s="26"/>
+      <c r="AY2" s="26"/>
+      <c r="AZ2" s="26"/>
+      <c r="BA2" s="26"/>
+      <c r="BB2" s="26"/>
+      <c r="BC2" s="26"/>
+      <c r="BD2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="BF2" s="25"/>
-      <c r="BG2" s="25"/>
-      <c r="BH2" s="25"/>
-      <c r="BI2" s="25"/>
-      <c r="BJ2" s="25" t="s">
+      <c r="BE2" s="26"/>
+      <c r="BF2" s="26"/>
+      <c r="BG2" s="26"/>
+      <c r="BH2" s="26"/>
+      <c r="BI2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="BK2" s="25"/>
-      <c r="BL2" s="25"/>
-      <c r="BM2" s="25"/>
-      <c r="BN2" s="5" t="s">
+      <c r="BJ2" s="26"/>
+      <c r="BK2" s="26"/>
+      <c r="BL2" s="26"/>
+      <c r="BM2" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>200000</v>
       </c>
@@ -2551,127 +2588,124 @@
         <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="26" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="26" t="s">
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="26" t="s">
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="26" t="s">
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="27"/>
-      <c r="AI3" s="27"/>
-      <c r="AJ3" s="28"/>
-      <c r="AK3" s="26" t="s">
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="AL3" s="27"/>
-      <c r="AM3" s="27"/>
-      <c r="AN3" s="27"/>
-      <c r="AO3" s="28"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="29"/>
+      <c r="AO3" s="3">
+        <v>0</v>
+      </c>
       <c r="AP3" s="3">
         <v>0</v>
       </c>
-      <c r="AQ3" s="3">
-        <v>0</v>
+      <c r="AQ3" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="AR3" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AS3" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AT3" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AU3" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AV3" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AW3" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AX3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB3" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="BC3" s="31"/>
+      <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AY3" s="10" t="s">
+      <c r="BE3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AZ3" s="10" t="s">
+      <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BA3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="BB3" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="BC3" s="29" t="s">
+      <c r="BG3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BD3" s="29"/>
-      <c r="BE3" s="10" t="s">
+      <c r="BH3" s="31"/>
+      <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="BF3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="BG3" s="10" t="s">
+      <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BH3" s="29" t="s">
+      <c r="BK3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BI3" s="29"/>
-      <c r="BJ3" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="BK3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="BL3" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="BM3" s="29"/>
-      <c r="BN3" s="10" t="s">
+      <c r="BL3" s="31"/>
+      <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2690,70 +2724,70 @@
       <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="29"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3">
+        <v>5</v>
+      </c>
+      <c r="AQ4" s="10" t="s">
         <v>1</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="R4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="W4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="28"/>
-      <c r="AK4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="28"/>
-      <c r="AP4" s="3"/>
-      <c r="AQ4" s="3">
-        <v>5</v>
       </c>
       <c r="AR4" s="10" t="s">
         <v>1</v>
@@ -2789,10 +2823,10 @@
         <v>1</v>
       </c>
       <c r="BC4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD4" s="10" t="s">
         <v>1</v>
-      </c>
-      <c r="BD4" s="10" t="s">
-        <v>2</v>
       </c>
       <c r="BE4" s="10" t="s">
         <v>1</v>
@@ -2804,10 +2838,10 @@
         <v>1</v>
       </c>
       <c r="BH4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI4" s="10" t="s">
         <v>1</v>
-      </c>
-      <c r="BI4" s="10" t="s">
-        <v>2</v>
       </c>
       <c r="BJ4" s="10" t="s">
         <v>1</v>
@@ -2816,16 +2850,13 @@
         <v>1</v>
       </c>
       <c r="BL4" s="10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BM4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="BN4" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3">
@@ -2841,94 +2872,96 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="3">
+      <c r="K5" s="3">
         <v>5</v>
       </c>
+      <c r="L5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="M5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="26"/>
+      <c r="P5" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="S5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="3">
-        <v>7</v>
-      </c>
-      <c r="R5" s="3" t="s">
+      <c r="T5" s="26"/>
+      <c r="U5" s="3">
+        <v>13</v>
+      </c>
+      <c r="V5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T5" s="25" t="s">
+      <c r="X5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="U5" s="25"/>
-      <c r="V5" s="3">
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="3">
+        <v>9</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="3">
         <v>13</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="AG5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Y5" s="25" t="s">
+      <c r="AH5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="3">
+      <c r="AI5" s="26"/>
+      <c r="AJ5" s="3">
         <v>9</v>
       </c>
-      <c r="AB5" s="3" t="s">
+      <c r="AK5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AL5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="25" t="s">
+      <c r="AM5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AE5" s="25"/>
-      <c r="AF5" s="3">
-        <v>13</v>
-      </c>
-      <c r="AG5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI5" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ5" s="25"/>
-      <c r="AK5" s="3">
-        <v>9</v>
-      </c>
-      <c r="AL5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN5" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="3">
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3">
         <v>10</v>
       </c>
+      <c r="AQ5" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AR5" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AS5" s="12" t="s">
         <v>68</v>
@@ -2942,60 +2975,57 @@
       <c r="AV5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AW5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AX5" s="10">
+      <c r="AW5" s="10">
         <v>9</v>
       </c>
-      <c r="AY5" s="12" t="s">
+      <c r="AX5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AZ5" s="10">
+      <c r="AY5" s="10">
         <v>15</v>
       </c>
-      <c r="BA5" s="12" t="s">
+      <c r="AZ5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="BB5" s="10">
+      <c r="BA5" s="10">
         <v>12</v>
       </c>
+      <c r="BB5" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="BC5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="BD5" s="10">
+        <v>9</v>
+      </c>
+      <c r="BE5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF5" s="10">
+        <v>15</v>
+      </c>
+      <c r="BG5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="BD5" s="10" t="s">
+      <c r="BH5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="BE5" s="10">
+      <c r="BI5" s="10">
         <v>9</v>
       </c>
-      <c r="BF5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG5" s="10">
+      <c r="BJ5" s="10">
         <v>15</v>
       </c>
-      <c r="BH5" s="10" t="s">
+      <c r="BK5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="BI5" s="10" t="s">
+      <c r="BL5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="BJ5" s="10">
-        <v>9</v>
-      </c>
-      <c r="BK5" s="10">
-        <v>15</v>
-      </c>
-      <c r="BL5" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="BM5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="BN5" s="10"/>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="BM5" s="10"/>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -3011,92 +3041,92 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="M6" s="3" t="s">
         <v>63</v>
       </c>
       <c r="N6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="3"/>
       <c r="R6" s="3" t="s">
         <v>63</v>
       </c>
       <c r="S6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V6" s="3"/>
       <c r="W6" s="3" t="s">
         <v>63</v>
       </c>
       <c r="X6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Y6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA6" s="3"/>
       <c r="AB6" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AC6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AD6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF6" s="3"/>
       <c r="AG6" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AH6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AI6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK6" s="3"/>
       <c r="AL6" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AM6" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="AN6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AP6" s="3"/>
-      <c r="AQ6" s="3">
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3">
         <v>15</v>
       </c>
+      <c r="AQ6" s="10"/>
       <c r="AR6" s="10"/>
       <c r="AS6" s="10"/>
       <c r="AT6" s="10"/>
@@ -3108,26 +3138,25 @@
       <c r="AZ6" s="10"/>
       <c r="BA6" s="10"/>
       <c r="BB6" s="10"/>
-      <c r="BC6" s="10"/>
-      <c r="BD6" s="10" t="s">
+      <c r="BC6" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="BD6" s="10"/>
       <c r="BE6" s="10"/>
       <c r="BF6" s="10"/>
       <c r="BG6" s="10"/>
-      <c r="BH6" s="10"/>
-      <c r="BI6" s="10" t="s">
+      <c r="BH6" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="BI6" s="10"/>
       <c r="BJ6" s="10"/>
       <c r="BK6" s="10"/>
-      <c r="BL6" s="10"/>
-      <c r="BM6" s="10" t="s">
+      <c r="BL6" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="BN6" s="10"/>
-    </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="BM6" s="10"/>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -3141,80 +3170,80 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="N7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U7" s="3" t="s">
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="X7" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="Y7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="Z7" s="3" t="s">
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC7" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="AD7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AE7" s="3" t="s">
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH7" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="AI7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AJ7" s="3" t="s">
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM7" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="AN7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AO7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP7" s="3"/>
-      <c r="AQ7" s="3">
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3">
         <v>20</v>
       </c>
+      <c r="AQ7" s="10"/>
       <c r="AR7" s="10"/>
       <c r="AS7" s="10"/>
       <c r="AT7" s="10"/>
@@ -3226,26 +3255,25 @@
       <c r="AZ7" s="10"/>
       <c r="BA7" s="10"/>
       <c r="BB7" s="10"/>
-      <c r="BC7" s="10"/>
-      <c r="BD7" s="10" t="s">
+      <c r="BC7" s="10" t="s">
         <v>74</v>
       </c>
+      <c r="BD7" s="10"/>
       <c r="BE7" s="10"/>
       <c r="BF7" s="10"/>
       <c r="BG7" s="10"/>
-      <c r="BH7" s="10"/>
-      <c r="BI7" s="10" t="s">
+      <c r="BH7" s="10" t="s">
         <v>74</v>
       </c>
+      <c r="BI7" s="10"/>
       <c r="BJ7" s="10"/>
       <c r="BK7" s="10"/>
-      <c r="BL7" s="10"/>
-      <c r="BM7" s="10" t="s">
+      <c r="BL7" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="BN7" s="10"/>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="BM7" s="10"/>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -3259,68 +3287,68 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="N8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="O8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
+      <c r="S8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="T8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U8" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
+      <c r="X8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="Y8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Z8" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
+      <c r="AC8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="AD8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AE8" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
+      <c r="AH8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="AI8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AJ8" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
-      <c r="AM8" s="3"/>
+      <c r="AM8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="AN8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AO8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP8" s="3"/>
-      <c r="AQ8" s="3">
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3">
         <v>25</v>
       </c>
+      <c r="AQ8" s="10"/>
       <c r="AR8" s="10"/>
       <c r="AS8" s="10"/>
       <c r="AT8" s="10"/>
@@ -3332,26 +3360,25 @@
       <c r="AZ8" s="10"/>
       <c r="BA8" s="10"/>
       <c r="BB8" s="10"/>
-      <c r="BC8" s="10"/>
-      <c r="BD8" s="10" t="s">
+      <c r="BC8" s="10" t="s">
         <v>75</v>
       </c>
+      <c r="BD8" s="10"/>
       <c r="BE8" s="10"/>
       <c r="BF8" s="10"/>
       <c r="BG8" s="10"/>
-      <c r="BH8" s="10"/>
-      <c r="BI8" s="10" t="s">
+      <c r="BH8" s="10" t="s">
         <v>75</v>
       </c>
+      <c r="BI8" s="10"/>
       <c r="BJ8" s="10"/>
       <c r="BK8" s="10"/>
-      <c r="BL8" s="10"/>
-      <c r="BM8" s="10" t="s">
+      <c r="BL8" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="BN8" s="10"/>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="BM8" s="10"/>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3">
@@ -3365,66 +3392,66 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="O9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
+      <c r="S9" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="T9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="U9" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
+      <c r="X9" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="Y9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Z9" s="3" t="s">
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
       <c r="AD9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AE9" s="3" t="s">
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
       <c r="AI9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AJ9" s="3" t="s">
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="3"/>
       <c r="AN9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AO9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP9" s="5"/>
-      <c r="AQ9" s="3">
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="3">
         <v>30</v>
       </c>
+      <c r="AQ9" s="10"/>
       <c r="AR9" s="10"/>
       <c r="AS9" s="10"/>
       <c r="AT9" s="10"/>
@@ -3436,26 +3463,25 @@
       <c r="AZ9" s="10"/>
       <c r="BA9" s="10"/>
       <c r="BB9" s="10"/>
-      <c r="BC9" s="10"/>
-      <c r="BD9" s="10" t="s">
+      <c r="BC9" s="10" t="s">
         <v>76</v>
       </c>
+      <c r="BD9" s="10"/>
       <c r="BE9" s="10"/>
       <c r="BF9" s="10"/>
       <c r="BG9" s="10"/>
-      <c r="BH9" s="10"/>
-      <c r="BI9" s="10" t="s">
+      <c r="BH9" s="10" t="s">
         <v>76</v>
       </c>
+      <c r="BI9" s="10"/>
       <c r="BJ9" s="10"/>
       <c r="BK9" s="10"/>
-      <c r="BL9" s="10"/>
-      <c r="BM9" s="10" t="s">
+      <c r="BL9" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="BN9" s="10"/>
-    </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="BM9" s="10"/>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -3470,65 +3496,65 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="N10" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="O10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="5"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
       <c r="T10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="U10" s="5"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="V10" s="5"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
       <c r="Y10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Z10" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
+      <c r="AC10" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="AD10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AE10" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
+      <c r="AH10" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="AI10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AJ10" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
+      <c r="AM10" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="AN10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AO10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AP10" s="3"/>
-      <c r="AQ10" s="3">
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3">
         <v>35</v>
       </c>
+      <c r="AQ10" s="3"/>
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
       <c r="AT10" s="3"/>
@@ -3551,9 +3577,8 @@
       <c r="BK10" s="3"/>
       <c r="BL10" s="3"/>
       <c r="BM10" s="3"/>
-      <c r="BN10" s="3"/>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -3569,64 +3594,64 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="3"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="O11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="3"/>
       <c r="T11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="3" t="s">
+      <c r="U11" s="3"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V11" s="3"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="3"/>
       <c r="Y11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z11" s="3" t="s">
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="3"/>
       <c r="AD11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AE11" s="3" t="s">
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="5"/>
-      <c r="AH11" s="3"/>
       <c r="AI11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AJ11" s="3" t="s">
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AK11" s="3"/>
-      <c r="AL11" s="5"/>
-      <c r="AM11" s="3"/>
       <c r="AN11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AO11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP11" s="3"/>
-      <c r="AQ11" s="3">
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3">
         <v>40</v>
       </c>
+      <c r="AQ11" s="3"/>
       <c r="AR11" s="3"/>
       <c r="AS11" s="3"/>
       <c r="AT11" s="3"/>
@@ -3649,9 +3674,8 @@
       <c r="BK11" s="3"/>
       <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
-      <c r="BN11" s="3"/>
-    </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3">
@@ -3666,65 +3690,65 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="O12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
+      <c r="S12" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="T12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="U12" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
+      <c r="X12" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="Y12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Z12" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
+      <c r="AC12" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AD12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AE12" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
+      <c r="AH12" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AI12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AJ12" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
-      <c r="AM12" s="3"/>
+      <c r="AM12" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AN12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AO12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP12" s="5"/>
-      <c r="AQ12" s="3">
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="3">
         <v>45</v>
       </c>
+      <c r="AQ12" s="3"/>
       <c r="AR12" s="3"/>
       <c r="AS12" s="3"/>
       <c r="AT12" s="3"/>
@@ -3747,9 +3771,8 @@
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
-      <c r="BN12" s="3"/>
-    </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3764,65 +3787,65 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="3"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="N13" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="O13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="5"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
       <c r="T13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="U13" s="3" t="s">
+      <c r="U13" s="5"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="V13" s="5"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
       <c r="Y13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Z13" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
+      <c r="AC13" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="AD13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AE13" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
+      <c r="AH13" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="AI13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AJ13" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
-      <c r="AM13" s="3"/>
+      <c r="AM13" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="AN13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AO13" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AP13" s="3"/>
-      <c r="AQ13" s="3">
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3">
         <v>50</v>
       </c>
+      <c r="AQ13" s="3"/>
       <c r="AR13" s="3"/>
       <c r="AS13" s="3"/>
       <c r="AT13" s="3"/>
@@ -3845,9 +3868,8 @@
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
-      <c r="BN13" s="3"/>
-    </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3">
@@ -3862,65 +3884,65 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="O14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="3"/>
       <c r="T14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="U14" s="3" t="s">
+      <c r="U14" s="3"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="V14" s="3"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="3"/>
       <c r="Y14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Z14" s="3" t="s">
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="3"/>
       <c r="AD14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AE14" s="3" t="s">
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="5"/>
-      <c r="AH14" s="3"/>
       <c r="AI14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AJ14" s="3" t="s">
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AK14" s="3"/>
-      <c r="AL14" s="5"/>
-      <c r="AM14" s="3"/>
       <c r="AN14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AO14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP14" s="5"/>
-      <c r="AQ14" s="3">
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="3">
         <v>55</v>
       </c>
+      <c r="AQ14" s="3"/>
       <c r="AR14" s="3"/>
       <c r="AS14" s="3"/>
       <c r="AT14" s="3"/>
@@ -3943,9 +3965,8 @@
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
-      <c r="BN14" s="3"/>
-    </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -3960,65 +3981,65 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="3"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="N15" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="O15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" s="5"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
       <c r="T15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="U15" s="3" t="s">
+      <c r="U15" s="5"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="V15" s="5"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
       <c r="Y15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Z15" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
+      <c r="AC15" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AD15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AE15" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
+      <c r="AH15" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AI15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AJ15" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="AJ15" s="3"/>
       <c r="AK15" s="3"/>
       <c r="AL15" s="3"/>
-      <c r="AM15" s="3"/>
+      <c r="AM15" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AN15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AO15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP15" s="3"/>
-      <c r="AQ15" s="3">
+      <c r="AO15" s="3"/>
+      <c r="AP15" s="3">
         <v>60</v>
       </c>
+      <c r="AQ15" s="3"/>
       <c r="AR15" s="3"/>
       <c r="AS15" s="3"/>
       <c r="AT15" s="3"/>
@@ -4041,9 +4062,8 @@
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
-      <c r="BN15" s="3"/>
-    </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -4059,64 +4079,64 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="3"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="O16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="3"/>
       <c r="T16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="U16" s="3" t="s">
+      <c r="U16" s="3"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="V16" s="3"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="3"/>
       <c r="Y16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Z16" s="3" t="s">
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="3"/>
       <c r="AD16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AE16" s="3" t="s">
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="5"/>
-      <c r="AH16" s="3"/>
       <c r="AI16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AJ16" s="3" t="s">
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AK16" s="3"/>
-      <c r="AL16" s="5"/>
-      <c r="AM16" s="3"/>
       <c r="AN16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AO16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP16" s="3"/>
-      <c r="AQ16" s="3">
+      <c r="AO16" s="3"/>
+      <c r="AP16" s="3">
         <v>65</v>
       </c>
+      <c r="AQ16" s="3"/>
       <c r="AR16" s="3"/>
       <c r="AS16" s="3"/>
       <c r="AT16" s="3"/>
@@ -4139,9 +4159,8 @@
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
       <c r="BM16" s="3"/>
-      <c r="BN16" s="3"/>
-    </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -4159,62 +4178,62 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="O17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P17" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
+      <c r="S17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="T17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="U17" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
+      <c r="X17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="Y17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Z17" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
+      <c r="AC17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AD17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AE17" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
+      <c r="AH17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AI17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AJ17" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
       <c r="AL17" s="3"/>
-      <c r="AM17" s="3"/>
+      <c r="AM17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AN17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AO17" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP17" s="3"/>
-      <c r="AQ17" s="3">
+      <c r="AO17" s="3"/>
+      <c r="AP17" s="3">
         <v>70</v>
       </c>
+      <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
       <c r="AT17" s="3"/>
@@ -4237,9 +4256,8 @@
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
-      <c r="BN17" s="3"/>
-    </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -4257,62 +4275,62 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="O18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P18" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="S18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="T18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="U18" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
+      <c r="X18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="Y18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Z18" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
+      <c r="AC18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AD18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AE18" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
+      <c r="AH18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AI18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AJ18" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
       <c r="AL18" s="3"/>
-      <c r="AM18" s="3"/>
+      <c r="AM18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="AN18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AO18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP18" s="3"/>
-      <c r="AQ18" s="3">
+      <c r="AO18" s="3"/>
+      <c r="AP18" s="3">
         <v>75</v>
       </c>
+      <c r="AQ18" s="3"/>
       <c r="AR18" s="3"/>
       <c r="AS18" s="3"/>
       <c r="AT18" s="3"/>
@@ -4335,9 +4353,8 @@
       <c r="BK18" s="3"/>
       <c r="BL18" s="3"/>
       <c r="BM18" s="3"/>
-      <c r="BN18" s="3"/>
-    </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -4355,62 +4372,62 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="N19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="O19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P19" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="S19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="T19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="U19" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
+      <c r="X19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="Y19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Z19" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
+      <c r="AC19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AD19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AE19" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
+      <c r="AH19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AI19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AJ19" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="AJ19" s="3"/>
       <c r="AK19" s="3"/>
       <c r="AL19" s="3"/>
-      <c r="AM19" s="3"/>
+      <c r="AM19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="AN19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AO19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP19" s="3"/>
-      <c r="AQ19" s="3">
+      <c r="AO19" s="3"/>
+      <c r="AP19" s="3">
         <v>80</v>
       </c>
+      <c r="AQ19" s="3"/>
       <c r="AR19" s="3"/>
       <c r="AS19" s="3"/>
       <c r="AT19" s="3"/>
@@ -4433,9 +4450,8 @@
       <c r="BK19" s="3"/>
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
-      <c r="BN19" s="3"/>
-    </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -4481,10 +4497,10 @@
       <c r="AM20" s="3"/>
       <c r="AN20" s="3"/>
       <c r="AO20" s="3"/>
-      <c r="AP20" s="3"/>
-      <c r="AQ20" s="3">
+      <c r="AP20" s="3">
         <v>85</v>
       </c>
+      <c r="AQ20" s="3"/>
       <c r="AR20" s="3"/>
       <c r="AS20" s="3"/>
       <c r="AT20" s="3"/>
@@ -4507,9 +4523,8 @@
       <c r="BK20" s="3"/>
       <c r="BL20" s="3"/>
       <c r="BM20" s="3"/>
-      <c r="BN20" s="3"/>
-    </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -4555,10 +4570,10 @@
       <c r="AM21" s="3"/>
       <c r="AN21" s="3"/>
       <c r="AO21" s="3"/>
-      <c r="AP21" s="3"/>
-      <c r="AQ21" s="3">
+      <c r="AP21" s="3">
         <v>90</v>
       </c>
+      <c r="AQ21" s="3"/>
       <c r="AR21" s="3"/>
       <c r="AS21" s="3"/>
       <c r="AT21" s="3"/>
@@ -4581,9 +4596,8 @@
       <c r="BK21" s="3"/>
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
-      <c r="BN21" s="3"/>
-    </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -4629,10 +4643,10 @@
       <c r="AM22" s="3"/>
       <c r="AN22" s="3"/>
       <c r="AO22" s="3"/>
-      <c r="AP22" s="3"/>
-      <c r="AQ22" s="3">
+      <c r="AP22" s="3">
         <v>95</v>
       </c>
+      <c r="AQ22" s="3"/>
       <c r="AR22" s="3"/>
       <c r="AS22" s="3"/>
       <c r="AT22" s="3"/>
@@ -4655,9 +4669,8 @@
       <c r="BK22" s="3"/>
       <c r="BL22" s="3"/>
       <c r="BM22" s="3"/>
-      <c r="BN22" s="3"/>
-    </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -4703,10 +4716,10 @@
       <c r="AM23" s="3"/>
       <c r="AN23" s="3"/>
       <c r="AO23" s="3"/>
-      <c r="AP23" s="3"/>
-      <c r="AQ23" s="3">
+      <c r="AP23" s="3">
         <v>100</v>
       </c>
+      <c r="AQ23" s="3"/>
       <c r="AR23" s="3"/>
       <c r="AS23" s="3"/>
       <c r="AT23" s="3"/>
@@ -4729,9 +4742,8 @@
       <c r="BK23" s="3"/>
       <c r="BL23" s="3"/>
       <c r="BM23" s="3"/>
-      <c r="BN23" s="3"/>
-    </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -4777,10 +4789,10 @@
       <c r="AM24" s="3"/>
       <c r="AN24" s="3"/>
       <c r="AO24" s="3"/>
-      <c r="AP24" s="3"/>
-      <c r="AQ24" s="3">
+      <c r="AP24" s="3">
         <v>105</v>
       </c>
+      <c r="AQ24" s="3"/>
       <c r="AR24" s="3"/>
       <c r="AS24" s="3"/>
       <c r="AT24" s="3"/>
@@ -4803,9 +4815,8 @@
       <c r="BK24" s="3"/>
       <c r="BL24" s="3"/>
       <c r="BM24" s="3"/>
-      <c r="BN24" s="3"/>
-    </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3">
@@ -4851,10 +4862,10 @@
       <c r="AM25" s="3"/>
       <c r="AN25" s="3"/>
       <c r="AO25" s="3"/>
-      <c r="AP25" s="3"/>
-      <c r="AQ25" s="3">
+      <c r="AP25" s="3">
         <v>110</v>
       </c>
+      <c r="AQ25" s="3"/>
       <c r="AR25" s="3"/>
       <c r="AS25" s="3"/>
       <c r="AT25" s="3"/>
@@ -4877,9 +4888,8 @@
       <c r="BK25" s="3"/>
       <c r="BL25" s="3"/>
       <c r="BM25" s="3"/>
-      <c r="BN25" s="3"/>
-    </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3">
@@ -4925,10 +4935,10 @@
       <c r="AM26" s="3"/>
       <c r="AN26" s="3"/>
       <c r="AO26" s="3"/>
-      <c r="AP26" s="3"/>
-      <c r="AQ26" s="3">
+      <c r="AP26" s="3">
         <v>115</v>
       </c>
+      <c r="AQ26" s="3"/>
       <c r="AR26" s="3"/>
       <c r="AS26" s="3"/>
       <c r="AT26" s="3"/>
@@ -4951,9 +4961,8 @@
       <c r="BK26" s="3"/>
       <c r="BL26" s="3"/>
       <c r="BM26" s="3"/>
-      <c r="BN26" s="3"/>
-    </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
@@ -4999,10 +5008,10 @@
       <c r="AM27" s="3"/>
       <c r="AN27" s="3"/>
       <c r="AO27" s="3"/>
-      <c r="AP27" s="3"/>
-      <c r="AQ27" s="3">
+      <c r="AP27" s="3">
         <v>120</v>
       </c>
+      <c r="AQ27" s="3"/>
       <c r="AR27" s="3"/>
       <c r="AS27" s="3"/>
       <c r="AT27" s="3"/>
@@ -5025,9 +5034,8 @@
       <c r="BK27" s="3"/>
       <c r="BL27" s="3"/>
       <c r="BM27" s="3"/>
-      <c r="BN27" s="3"/>
-    </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
@@ -5073,10 +5081,10 @@
       <c r="AM28" s="3"/>
       <c r="AN28" s="3"/>
       <c r="AO28" s="3"/>
-      <c r="AP28" s="3"/>
-      <c r="AQ28" s="3">
+      <c r="AP28" s="3">
         <v>125</v>
       </c>
+      <c r="AQ28" s="3"/>
       <c r="AR28" s="3"/>
       <c r="AS28" s="3"/>
       <c r="AT28" s="3"/>
@@ -5099,9 +5107,8 @@
       <c r="BK28" s="3"/>
       <c r="BL28" s="3"/>
       <c r="BM28" s="3"/>
-      <c r="BN28" s="3"/>
-    </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
@@ -5147,10 +5154,10 @@
       <c r="AM29" s="3"/>
       <c r="AN29" s="3"/>
       <c r="AO29" s="3"/>
-      <c r="AP29" s="3"/>
-      <c r="AQ29" s="3">
+      <c r="AP29" s="3">
         <v>130</v>
       </c>
+      <c r="AQ29" s="3"/>
       <c r="AR29" s="3"/>
       <c r="AS29" s="3"/>
       <c r="AT29" s="3"/>
@@ -5173,9 +5180,8 @@
       <c r="BK29" s="3"/>
       <c r="BL29" s="3"/>
       <c r="BM29" s="3"/>
-      <c r="BN29" s="3"/>
-    </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
@@ -5221,10 +5227,10 @@
       <c r="AM30" s="3"/>
       <c r="AN30" s="3"/>
       <c r="AO30" s="3"/>
-      <c r="AP30" s="3"/>
-      <c r="AQ30" s="3">
+      <c r="AP30" s="3">
         <v>135</v>
       </c>
+      <c r="AQ30" s="3"/>
       <c r="AR30" s="3"/>
       <c r="AS30" s="3"/>
       <c r="AT30" s="3"/>
@@ -5247,9 +5253,8 @@
       <c r="BK30" s="3"/>
       <c r="BL30" s="3"/>
       <c r="BM30" s="3"/>
-      <c r="BN30" s="3"/>
-    </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
@@ -5295,10 +5300,10 @@
       <c r="AM31" s="3"/>
       <c r="AN31" s="3"/>
       <c r="AO31" s="3"/>
-      <c r="AP31" s="3"/>
-      <c r="AQ31" s="3">
+      <c r="AP31" s="3">
         <v>140</v>
       </c>
+      <c r="AQ31" s="3"/>
       <c r="AR31" s="3"/>
       <c r="AS31" s="3"/>
       <c r="AT31" s="3"/>
@@ -5321,9 +5326,8 @@
       <c r="BK31" s="3"/>
       <c r="BL31" s="3"/>
       <c r="BM31" s="3"/>
-      <c r="BN31" s="3"/>
-    </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
@@ -5369,10 +5373,10 @@
       <c r="AM32" s="3"/>
       <c r="AN32" s="3"/>
       <c r="AO32" s="3"/>
-      <c r="AP32" s="3"/>
-      <c r="AQ32" s="3">
+      <c r="AP32" s="3">
         <v>145</v>
       </c>
+      <c r="AQ32" s="3"/>
       <c r="AR32" s="3"/>
       <c r="AS32" s="3"/>
       <c r="AT32" s="3"/>
@@ -5395,9 +5399,8 @@
       <c r="BK32" s="3"/>
       <c r="BL32" s="3"/>
       <c r="BM32" s="3"/>
-      <c r="BN32" s="3"/>
-    </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3">
@@ -5443,10 +5446,10 @@
       <c r="AM33" s="3"/>
       <c r="AN33" s="3"/>
       <c r="AO33" s="3"/>
-      <c r="AP33" s="3"/>
-      <c r="AQ33" s="3">
+      <c r="AP33" s="3">
         <v>150</v>
       </c>
+      <c r="AQ33" s="3"/>
       <c r="AR33" s="3"/>
       <c r="AS33" s="3"/>
       <c r="AT33" s="3"/>
@@ -5469,9 +5472,8 @@
       <c r="BK33" s="3"/>
       <c r="BL33" s="3"/>
       <c r="BM33" s="3"/>
-      <c r="BN33" s="3"/>
-    </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
@@ -5517,10 +5519,10 @@
       <c r="AM34" s="3"/>
       <c r="AN34" s="3"/>
       <c r="AO34" s="3"/>
-      <c r="AP34" s="3"/>
-      <c r="AQ34" s="3">
+      <c r="AP34" s="3">
         <v>155</v>
       </c>
+      <c r="AQ34" s="3"/>
       <c r="AR34" s="3"/>
       <c r="AS34" s="3"/>
       <c r="AT34" s="3"/>
@@ -5543,9 +5545,8 @@
       <c r="BK34" s="3"/>
       <c r="BL34" s="3"/>
       <c r="BM34" s="3"/>
-      <c r="BN34" s="3"/>
-    </row>
-    <row r="35" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
@@ -5591,10 +5592,10 @@
       <c r="AM35" s="3"/>
       <c r="AN35" s="3"/>
       <c r="AO35" s="3"/>
-      <c r="AP35" s="3"/>
-      <c r="AQ35" s="3">
+      <c r="AP35" s="3">
         <v>160</v>
       </c>
+      <c r="AQ35" s="3"/>
       <c r="AR35" s="3"/>
       <c r="AS35" s="3"/>
       <c r="AT35" s="3"/>
@@ -5617,9 +5618,8 @@
       <c r="BK35" s="3"/>
       <c r="BL35" s="3"/>
       <c r="BM35" s="3"/>
-      <c r="BN35" s="3"/>
-    </row>
-    <row r="36" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
@@ -5663,10 +5663,10 @@
       <c r="AM36" s="3"/>
       <c r="AN36" s="3"/>
       <c r="AO36" s="3"/>
-      <c r="AP36" s="3"/>
-      <c r="AQ36" s="3">
+      <c r="AP36" s="3">
         <v>165</v>
       </c>
+      <c r="AQ36" s="3"/>
       <c r="AR36" s="3"/>
       <c r="AS36" s="3"/>
       <c r="AT36" s="3"/>
@@ -5689,9 +5689,8 @@
       <c r="BK36" s="3"/>
       <c r="BL36" s="3"/>
       <c r="BM36" s="3"/>
-      <c r="BN36" s="3"/>
-    </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3">
@@ -5735,10 +5734,10 @@
       <c r="AM37" s="3"/>
       <c r="AN37" s="3"/>
       <c r="AO37" s="3"/>
-      <c r="AP37" s="3"/>
-      <c r="AQ37" s="3">
+      <c r="AP37" s="3">
         <v>170</v>
       </c>
+      <c r="AQ37" s="3"/>
       <c r="AR37" s="3"/>
       <c r="AS37" s="3"/>
       <c r="AT37" s="3"/>
@@ -5761,9 +5760,8 @@
       <c r="BK37" s="3"/>
       <c r="BL37" s="3"/>
       <c r="BM37" s="3"/>
-      <c r="BN37" s="3"/>
-    </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3">
@@ -5807,10 +5805,10 @@
       <c r="AM38" s="3"/>
       <c r="AN38" s="3"/>
       <c r="AO38" s="3"/>
-      <c r="AP38" s="3"/>
-      <c r="AQ38" s="3">
+      <c r="AP38" s="3">
         <v>175</v>
       </c>
+      <c r="AQ38" s="3"/>
       <c r="AR38" s="3"/>
       <c r="AS38" s="3"/>
       <c r="AT38" s="3"/>
@@ -5833,9 +5831,8 @@
       <c r="BK38" s="3"/>
       <c r="BL38" s="3"/>
       <c r="BM38" s="3"/>
-      <c r="BN38" s="3"/>
-    </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3">
@@ -5879,10 +5876,10 @@
       <c r="AM39" s="3"/>
       <c r="AN39" s="3"/>
       <c r="AO39" s="3"/>
-      <c r="AP39" s="3"/>
-      <c r="AQ39" s="3">
+      <c r="AP39" s="3">
         <v>180</v>
       </c>
+      <c r="AQ39" s="3"/>
       <c r="AR39" s="3"/>
       <c r="AS39" s="3"/>
       <c r="AT39" s="3"/>
@@ -5905,9 +5902,8 @@
       <c r="BK39" s="3"/>
       <c r="BL39" s="3"/>
       <c r="BM39" s="3"/>
-      <c r="BN39" s="3"/>
-    </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3">
@@ -5951,10 +5947,10 @@
       <c r="AM40" s="3"/>
       <c r="AN40" s="3"/>
       <c r="AO40" s="3"/>
-      <c r="AP40" s="3"/>
-      <c r="AQ40" s="3">
+      <c r="AP40" s="3">
         <v>185</v>
       </c>
+      <c r="AQ40" s="3"/>
       <c r="AR40" s="3"/>
       <c r="AS40" s="3"/>
       <c r="AT40" s="3"/>
@@ -5977,9 +5973,8 @@
       <c r="BK40" s="3"/>
       <c r="BL40" s="3"/>
       <c r="BM40" s="3"/>
-      <c r="BN40" s="3"/>
-    </row>
-    <row r="41" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3">
@@ -6023,10 +6018,10 @@
       <c r="AM41" s="3"/>
       <c r="AN41" s="3"/>
       <c r="AO41" s="3"/>
-      <c r="AP41" s="3"/>
-      <c r="AQ41" s="3">
+      <c r="AP41" s="3">
         <v>190</v>
       </c>
+      <c r="AQ41" s="3"/>
       <c r="AR41" s="3"/>
       <c r="AS41" s="3"/>
       <c r="AT41" s="3"/>
@@ -6049,9 +6044,8 @@
       <c r="BK41" s="3"/>
       <c r="BL41" s="3"/>
       <c r="BM41" s="3"/>
-      <c r="BN41" s="3"/>
-    </row>
-    <row r="42" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3">
@@ -6095,10 +6089,10 @@
       <c r="AM42" s="3"/>
       <c r="AN42" s="3"/>
       <c r="AO42" s="3"/>
-      <c r="AP42" s="3"/>
-      <c r="AQ42" s="3">
+      <c r="AP42" s="3">
         <v>195</v>
       </c>
+      <c r="AQ42" s="3"/>
       <c r="AR42" s="3"/>
       <c r="AS42" s="3"/>
       <c r="AT42" s="3"/>
@@ -6121,9 +6115,8 @@
       <c r="BK42" s="3"/>
       <c r="BL42" s="3"/>
       <c r="BM42" s="3"/>
-      <c r="BN42" s="3"/>
-    </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3">
@@ -6167,10 +6160,10 @@
       <c r="AM43" s="3"/>
       <c r="AN43" s="3"/>
       <c r="AO43" s="3"/>
-      <c r="AP43" s="3"/>
-      <c r="AQ43" s="3">
+      <c r="AP43" s="3">
         <v>200</v>
       </c>
+      <c r="AQ43" s="3"/>
       <c r="AR43" s="3"/>
       <c r="AS43" s="3"/>
       <c r="AT43" s="3"/>
@@ -6193,9 +6186,8 @@
       <c r="BK43" s="3"/>
       <c r="BL43" s="3"/>
       <c r="BM43" s="3"/>
-      <c r="BN43" s="3"/>
-    </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3">
@@ -6239,10 +6231,10 @@
       <c r="AM44" s="3"/>
       <c r="AN44" s="3"/>
       <c r="AO44" s="3"/>
-      <c r="AP44" s="3"/>
-      <c r="AQ44" s="3">
+      <c r="AP44" s="3">
         <v>205</v>
       </c>
+      <c r="AQ44" s="3"/>
       <c r="AR44" s="3"/>
       <c r="AS44" s="3"/>
       <c r="AT44" s="3"/>
@@ -6265,9 +6257,8 @@
       <c r="BK44" s="3"/>
       <c r="BL44" s="3"/>
       <c r="BM44" s="3"/>
-      <c r="BN44" s="3"/>
-    </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3">
@@ -6311,10 +6302,10 @@
       <c r="AM45" s="3"/>
       <c r="AN45" s="3"/>
       <c r="AO45" s="3"/>
-      <c r="AP45" s="3"/>
-      <c r="AQ45" s="3">
+      <c r="AP45" s="3">
         <v>210</v>
       </c>
+      <c r="AQ45" s="3"/>
       <c r="AR45" s="3"/>
       <c r="AS45" s="3"/>
       <c r="AT45" s="3"/>
@@ -6337,9 +6328,8 @@
       <c r="BK45" s="3"/>
       <c r="BL45" s="3"/>
       <c r="BM45" s="3"/>
-      <c r="BN45" s="3"/>
-    </row>
-    <row r="46" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
@@ -6383,10 +6373,10 @@
       <c r="AM46" s="3"/>
       <c r="AN46" s="3"/>
       <c r="AO46" s="3"/>
-      <c r="AP46" s="3"/>
-      <c r="AQ46" s="3">
+      <c r="AP46" s="3">
         <v>215</v>
       </c>
+      <c r="AQ46" s="3"/>
       <c r="AR46" s="3"/>
       <c r="AS46" s="3"/>
       <c r="AT46" s="3"/>
@@ -6409,9 +6399,8 @@
       <c r="BK46" s="3"/>
       <c r="BL46" s="3"/>
       <c r="BM46" s="3"/>
-      <c r="BN46" s="3"/>
-    </row>
-    <row r="47" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3">
@@ -6455,10 +6444,10 @@
       <c r="AM47" s="3"/>
       <c r="AN47" s="3"/>
       <c r="AO47" s="3"/>
-      <c r="AP47" s="3"/>
-      <c r="AQ47" s="3">
+      <c r="AP47" s="3">
         <v>220</v>
       </c>
+      <c r="AQ47" s="3"/>
       <c r="AR47" s="3"/>
       <c r="AS47" s="3"/>
       <c r="AT47" s="3"/>
@@ -6481,9 +6470,8 @@
       <c r="BK47" s="3"/>
       <c r="BL47" s="3"/>
       <c r="BM47" s="3"/>
-      <c r="BN47" s="3"/>
-    </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3">
@@ -6527,10 +6515,10 @@
       <c r="AM48" s="3"/>
       <c r="AN48" s="3"/>
       <c r="AO48" s="3"/>
-      <c r="AP48" s="3"/>
-      <c r="AQ48" s="3">
+      <c r="AP48" s="3">
         <v>225</v>
       </c>
+      <c r="AQ48" s="3"/>
       <c r="AR48" s="3"/>
       <c r="AS48" s="3"/>
       <c r="AT48" s="3"/>
@@ -6553,9 +6541,8 @@
       <c r="BK48" s="3"/>
       <c r="BL48" s="3"/>
       <c r="BM48" s="3"/>
-      <c r="BN48" s="3"/>
-    </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3">
@@ -6599,10 +6586,10 @@
       <c r="AM49" s="3"/>
       <c r="AN49" s="3"/>
       <c r="AO49" s="3"/>
-      <c r="AP49" s="3"/>
-      <c r="AQ49" s="3">
+      <c r="AP49" s="3">
         <v>230</v>
       </c>
+      <c r="AQ49" s="3"/>
       <c r="AR49" s="3"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="3"/>
@@ -6625,9 +6612,8 @@
       <c r="BK49" s="3"/>
       <c r="BL49" s="3"/>
       <c r="BM49" s="3"/>
-      <c r="BN49" s="3"/>
-    </row>
-    <row r="50" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3">
@@ -6671,10 +6657,10 @@
       <c r="AM50" s="3"/>
       <c r="AN50" s="3"/>
       <c r="AO50" s="3"/>
-      <c r="AP50" s="3"/>
-      <c r="AQ50" s="3">
+      <c r="AP50" s="3">
         <v>235</v>
       </c>
+      <c r="AQ50" s="3"/>
       <c r="AR50" s="3"/>
       <c r="AS50" s="3"/>
       <c r="AT50" s="3"/>
@@ -6697,9 +6683,8 @@
       <c r="BK50" s="3"/>
       <c r="BL50" s="3"/>
       <c r="BM50" s="3"/>
-      <c r="BN50" s="3"/>
-    </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3">
@@ -6743,10 +6728,10 @@
       <c r="AM51" s="3"/>
       <c r="AN51" s="3"/>
       <c r="AO51" s="3"/>
-      <c r="AP51" s="3"/>
-      <c r="AQ51" s="3">
+      <c r="AP51" s="3">
         <v>240</v>
       </c>
+      <c r="AQ51" s="3"/>
       <c r="AR51" s="3"/>
       <c r="AS51" s="3"/>
       <c r="AT51" s="3"/>
@@ -6769,9 +6754,8 @@
       <c r="BK51" s="3"/>
       <c r="BL51" s="3"/>
       <c r="BM51" s="3"/>
-      <c r="BN51" s="3"/>
-    </row>
-    <row r="52" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3">
@@ -6815,10 +6799,10 @@
       <c r="AM52" s="3"/>
       <c r="AN52" s="3"/>
       <c r="AO52" s="3"/>
-      <c r="AP52" s="3"/>
-      <c r="AQ52" s="3">
+      <c r="AP52" s="3">
         <v>245</v>
       </c>
+      <c r="AQ52" s="3"/>
       <c r="AR52" s="3"/>
       <c r="AS52" s="3"/>
       <c r="AT52" s="3"/>
@@ -6841,9 +6825,8 @@
       <c r="BK52" s="3"/>
       <c r="BL52" s="3"/>
       <c r="BM52" s="3"/>
-      <c r="BN52" s="3"/>
-    </row>
-    <row r="53" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6885,10 +6868,10 @@
       <c r="AM53" s="3"/>
       <c r="AN53" s="3"/>
       <c r="AO53" s="3"/>
-      <c r="AP53" s="3"/>
-      <c r="AQ53" s="3">
+      <c r="AP53" s="3">
         <v>250</v>
       </c>
+      <c r="AQ53" s="3"/>
       <c r="AR53" s="3"/>
       <c r="AS53" s="3"/>
       <c r="AT53" s="3"/>
@@ -6911,9 +6894,8 @@
       <c r="BK53" s="3"/>
       <c r="BL53" s="3"/>
       <c r="BM53" s="3"/>
-      <c r="BN53" s="3"/>
-    </row>
-    <row r="54" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6955,10 +6937,10 @@
       <c r="AM54" s="3"/>
       <c r="AN54" s="3"/>
       <c r="AO54" s="3"/>
-      <c r="AP54" s="3"/>
-      <c r="AQ54" s="3">
+      <c r="AP54" s="3">
         <v>255</v>
       </c>
+      <c r="AQ54" s="3"/>
       <c r="AR54" s="3"/>
       <c r="AS54" s="3"/>
       <c r="AT54" s="3"/>
@@ -6981,9 +6963,8 @@
       <c r="BK54" s="3"/>
       <c r="BL54" s="3"/>
       <c r="BM54" s="3"/>
-      <c r="BN54" s="3"/>
-    </row>
-    <row r="55" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -7025,10 +7006,10 @@
       <c r="AM55" s="3"/>
       <c r="AN55" s="3"/>
       <c r="AO55" s="3"/>
-      <c r="AP55" s="3"/>
-      <c r="AQ55" s="3">
+      <c r="AP55" s="3">
         <v>260</v>
       </c>
+      <c r="AQ55" s="3"/>
       <c r="AR55" s="3"/>
       <c r="AS55" s="3"/>
       <c r="AT55" s="3"/>
@@ -7051,9 +7032,8 @@
       <c r="BK55" s="3"/>
       <c r="BL55" s="3"/>
       <c r="BM55" s="3"/>
-      <c r="BN55" s="3"/>
-    </row>
-    <row r="56" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -7095,10 +7075,10 @@
       <c r="AM56" s="3"/>
       <c r="AN56" s="3"/>
       <c r="AO56" s="3"/>
-      <c r="AP56" s="3"/>
-      <c r="AQ56" s="3">
+      <c r="AP56" s="3">
         <v>265</v>
       </c>
+      <c r="AQ56" s="3"/>
       <c r="AR56" s="3"/>
       <c r="AS56" s="3"/>
       <c r="AT56" s="3"/>
@@ -7121,9 +7101,8 @@
       <c r="BK56" s="3"/>
       <c r="BL56" s="3"/>
       <c r="BM56" s="3"/>
-      <c r="BN56" s="3"/>
-    </row>
-    <row r="57" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -7165,10 +7144,10 @@
       <c r="AM57" s="3"/>
       <c r="AN57" s="3"/>
       <c r="AO57" s="3"/>
-      <c r="AP57" s="3"/>
-      <c r="AQ57" s="3">
+      <c r="AP57" s="3">
         <v>270</v>
       </c>
+      <c r="AQ57" s="3"/>
       <c r="AR57" s="3"/>
       <c r="AS57" s="3"/>
       <c r="AT57" s="3"/>
@@ -7191,9 +7170,8 @@
       <c r="BK57" s="3"/>
       <c r="BL57" s="3"/>
       <c r="BM57" s="3"/>
-      <c r="BN57" s="3"/>
-    </row>
-    <row r="58" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -7235,10 +7213,10 @@
       <c r="AM58" s="3"/>
       <c r="AN58" s="3"/>
       <c r="AO58" s="3"/>
-      <c r="AP58" s="3"/>
-      <c r="AQ58" s="3">
+      <c r="AP58" s="3">
         <v>275</v>
       </c>
+      <c r="AQ58" s="3"/>
       <c r="AR58" s="3"/>
       <c r="AS58" s="3"/>
       <c r="AT58" s="3"/>
@@ -7261,9 +7239,8 @@
       <c r="BK58" s="3"/>
       <c r="BL58" s="3"/>
       <c r="BM58" s="3"/>
-      <c r="BN58" s="3"/>
-    </row>
-    <row r="59" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -7305,10 +7282,10 @@
       <c r="AM59" s="3"/>
       <c r="AN59" s="3"/>
       <c r="AO59" s="3"/>
-      <c r="AP59" s="3"/>
-      <c r="AQ59" s="3">
+      <c r="AP59" s="3">
         <v>280</v>
       </c>
+      <c r="AQ59" s="3"/>
       <c r="AR59" s="3"/>
       <c r="AS59" s="3"/>
       <c r="AT59" s="3"/>
@@ -7331,9 +7308,8 @@
       <c r="BK59" s="3"/>
       <c r="BL59" s="3"/>
       <c r="BM59" s="3"/>
-      <c r="BN59" s="3"/>
-    </row>
-    <row r="60" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -7375,10 +7351,10 @@
       <c r="AM60" s="3"/>
       <c r="AN60" s="3"/>
       <c r="AO60" s="3"/>
-      <c r="AP60" s="3"/>
-      <c r="AQ60" s="3">
+      <c r="AP60" s="3">
         <v>285</v>
       </c>
+      <c r="AQ60" s="3"/>
       <c r="AR60" s="3"/>
       <c r="AS60" s="3"/>
       <c r="AT60" s="3"/>
@@ -7401,9 +7377,8 @@
       <c r="BK60" s="3"/>
       <c r="BL60" s="3"/>
       <c r="BM60" s="3"/>
-      <c r="BN60" s="3"/>
-    </row>
-    <row r="61" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -7445,10 +7420,10 @@
       <c r="AM61" s="3"/>
       <c r="AN61" s="3"/>
       <c r="AO61" s="3"/>
-      <c r="AP61" s="3"/>
-      <c r="AQ61" s="3">
+      <c r="AP61" s="3">
         <v>290</v>
       </c>
+      <c r="AQ61" s="3"/>
       <c r="AR61" s="3"/>
       <c r="AS61" s="3"/>
       <c r="AT61" s="3"/>
@@ -7471,9 +7446,8 @@
       <c r="BK61" s="3"/>
       <c r="BL61" s="3"/>
       <c r="BM61" s="3"/>
-      <c r="BN61" s="3"/>
-    </row>
-    <row r="62" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -7515,10 +7489,10 @@
       <c r="AM62" s="3"/>
       <c r="AN62" s="3"/>
       <c r="AO62" s="3"/>
-      <c r="AP62" s="3"/>
-      <c r="AQ62" s="3">
+      <c r="AP62" s="3">
         <v>295</v>
       </c>
+      <c r="AQ62" s="3"/>
       <c r="AR62" s="3"/>
       <c r="AS62" s="3"/>
       <c r="AT62" s="3"/>
@@ -7541,9 +7515,8 @@
       <c r="BK62" s="3"/>
       <c r="BL62" s="3"/>
       <c r="BM62" s="3"/>
-      <c r="BN62" s="3"/>
-    </row>
-    <row r="63" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -7585,10 +7558,10 @@
       <c r="AM63" s="3"/>
       <c r="AN63" s="3"/>
       <c r="AO63" s="3"/>
-      <c r="AP63" s="3"/>
-      <c r="AQ63" s="3">
+      <c r="AP63" s="3">
         <v>300</v>
       </c>
+      <c r="AQ63" s="3"/>
       <c r="AR63" s="3"/>
       <c r="AS63" s="3"/>
       <c r="AT63" s="3"/>
@@ -7611,9 +7584,8 @@
       <c r="BK63" s="3"/>
       <c r="BL63" s="3"/>
       <c r="BM63" s="3"/>
-      <c r="BN63" s="3"/>
-    </row>
-    <row r="64" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -7655,10 +7627,10 @@
       <c r="AM64" s="3"/>
       <c r="AN64" s="3"/>
       <c r="AO64" s="3"/>
-      <c r="AP64" s="3"/>
-      <c r="AQ64" s="3">
+      <c r="AP64" s="3">
         <v>305</v>
       </c>
+      <c r="AQ64" s="3"/>
       <c r="AR64" s="3"/>
       <c r="AS64" s="3"/>
       <c r="AT64" s="3"/>
@@ -7681,9 +7653,8 @@
       <c r="BK64" s="3"/>
       <c r="BL64" s="3"/>
       <c r="BM64" s="3"/>
-      <c r="BN64" s="3"/>
-    </row>
-    <row r="65" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -7725,10 +7696,10 @@
       <c r="AM65" s="3"/>
       <c r="AN65" s="3"/>
       <c r="AO65" s="3"/>
-      <c r="AP65" s="3"/>
-      <c r="AQ65" s="3">
+      <c r="AP65" s="3">
         <v>310</v>
       </c>
+      <c r="AQ65" s="3"/>
       <c r="AR65" s="3"/>
       <c r="AS65" s="3"/>
       <c r="AT65" s="3"/>
@@ -7751,9 +7722,8 @@
       <c r="BK65" s="3"/>
       <c r="BL65" s="3"/>
       <c r="BM65" s="3"/>
-      <c r="BN65" s="3"/>
-    </row>
-    <row r="66" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -7795,10 +7765,10 @@
       <c r="AM66" s="3"/>
       <c r="AN66" s="3"/>
       <c r="AO66" s="3"/>
-      <c r="AP66" s="3"/>
-      <c r="AQ66" s="3">
+      <c r="AP66" s="3">
         <v>315</v>
       </c>
+      <c r="AQ66" s="3"/>
       <c r="AR66" s="3"/>
       <c r="AS66" s="3"/>
       <c r="AT66" s="3"/>
@@ -7821,9 +7791,8 @@
       <c r="BK66" s="3"/>
       <c r="BL66" s="3"/>
       <c r="BM66" s="3"/>
-      <c r="BN66" s="3"/>
-    </row>
-    <row r="67" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -7865,10 +7834,10 @@
       <c r="AM67" s="3"/>
       <c r="AN67" s="3"/>
       <c r="AO67" s="3"/>
-      <c r="AP67" s="3"/>
-      <c r="AQ67" s="3">
+      <c r="AP67" s="3">
         <v>320</v>
       </c>
+      <c r="AQ67" s="3"/>
       <c r="AR67" s="3"/>
       <c r="AS67" s="3"/>
       <c r="AT67" s="3"/>
@@ -7891,9 +7860,8 @@
       <c r="BK67" s="3"/>
       <c r="BL67" s="3"/>
       <c r="BM67" s="3"/>
-      <c r="BN67" s="3"/>
-    </row>
-    <row r="68" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -7935,10 +7903,10 @@
       <c r="AM68" s="3"/>
       <c r="AN68" s="3"/>
       <c r="AO68" s="3"/>
-      <c r="AP68" s="3"/>
-      <c r="AQ68" s="3">
+      <c r="AP68" s="3">
         <v>325</v>
       </c>
+      <c r="AQ68" s="3"/>
       <c r="AR68" s="3"/>
       <c r="AS68" s="3"/>
       <c r="AT68" s="3"/>
@@ -7961,9 +7929,8 @@
       <c r="BK68" s="3"/>
       <c r="BL68" s="3"/>
       <c r="BM68" s="3"/>
-      <c r="BN68" s="3"/>
-    </row>
-    <row r="69" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -8005,10 +7972,10 @@
       <c r="AM69" s="3"/>
       <c r="AN69" s="3"/>
       <c r="AO69" s="3"/>
-      <c r="AP69" s="3"/>
-      <c r="AQ69" s="3">
+      <c r="AP69" s="3">
         <v>330</v>
       </c>
+      <c r="AQ69" s="3"/>
       <c r="AR69" s="3"/>
       <c r="AS69" s="3"/>
       <c r="AT69" s="3"/>
@@ -8031,9 +7998,8 @@
       <c r="BK69" s="3"/>
       <c r="BL69" s="3"/>
       <c r="BM69" s="3"/>
-      <c r="BN69" s="3"/>
-    </row>
-    <row r="70" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -8075,10 +8041,10 @@
       <c r="AM70" s="3"/>
       <c r="AN70" s="3"/>
       <c r="AO70" s="3"/>
-      <c r="AP70" s="3"/>
-      <c r="AQ70" s="3">
+      <c r="AP70" s="3">
         <v>335</v>
       </c>
+      <c r="AQ70" s="3"/>
       <c r="AR70" s="3"/>
       <c r="AS70" s="3"/>
       <c r="AT70" s="3"/>
@@ -8101,9 +8067,8 @@
       <c r="BK70" s="3"/>
       <c r="BL70" s="3"/>
       <c r="BM70" s="3"/>
-      <c r="BN70" s="3"/>
-    </row>
-    <row r="71" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -8145,10 +8110,10 @@
       <c r="AM71" s="3"/>
       <c r="AN71" s="3"/>
       <c r="AO71" s="3"/>
-      <c r="AP71" s="3"/>
-      <c r="AQ71" s="3">
+      <c r="AP71" s="3">
         <v>340</v>
       </c>
+      <c r="AQ71" s="3"/>
       <c r="AR71" s="3"/>
       <c r="AS71" s="3"/>
       <c r="AT71" s="3"/>
@@ -8171,9 +8136,8 @@
       <c r="BK71" s="3"/>
       <c r="BL71" s="3"/>
       <c r="BM71" s="3"/>
-      <c r="BN71" s="3"/>
-    </row>
-    <row r="72" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -8215,10 +8179,10 @@
       <c r="AM72" s="3"/>
       <c r="AN72" s="3"/>
       <c r="AO72" s="3"/>
-      <c r="AP72" s="3"/>
-      <c r="AQ72" s="3">
+      <c r="AP72" s="3">
         <v>345</v>
       </c>
+      <c r="AQ72" s="3"/>
       <c r="AR72" s="3"/>
       <c r="AS72" s="3"/>
       <c r="AT72" s="3"/>
@@ -8241,9 +8205,8 @@
       <c r="BK72" s="3"/>
       <c r="BL72" s="3"/>
       <c r="BM72" s="3"/>
-      <c r="BN72" s="3"/>
-    </row>
-    <row r="73" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -8285,10 +8248,10 @@
       <c r="AM73" s="3"/>
       <c r="AN73" s="3"/>
       <c r="AO73" s="3"/>
-      <c r="AP73" s="3"/>
-      <c r="AQ73" s="3">
+      <c r="AP73" s="3">
         <v>350</v>
       </c>
+      <c r="AQ73" s="3"/>
       <c r="AR73" s="3"/>
       <c r="AS73" s="3"/>
       <c r="AT73" s="3"/>
@@ -8311,9 +8274,8 @@
       <c r="BK73" s="3"/>
       <c r="BL73" s="3"/>
       <c r="BM73" s="3"/>
-      <c r="BN73" s="3"/>
-    </row>
-    <row r="74" spans="1:66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -8355,10 +8317,10 @@
       <c r="AM74" s="3"/>
       <c r="AN74" s="3"/>
       <c r="AO74" s="3"/>
-      <c r="AP74" s="3"/>
-      <c r="AQ74" s="3">
+      <c r="AP74" s="3">
         <v>355</v>
       </c>
+      <c r="AQ74" s="3"/>
       <c r="AR74" s="3"/>
       <c r="AS74" s="3"/>
       <c r="AT74" s="3"/>
@@ -8381,13 +8343,12 @@
       <c r="BK74" s="3"/>
       <c r="BL74" s="3"/>
       <c r="BM74" s="3"/>
-      <c r="BN74" s="3"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -8398,44 +8359,42 @@
       <c r="J143" s="8"/>
       <c r="K143" s="8"/>
       <c r="L143" s="8"/>
-      <c r="M143" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L2:AO2"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AG4:AJ4"/>
-    <mergeCell ref="AB4:AE4"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:BN1"/>
+  <mergeCells count="33">
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
+    <mergeCell ref="AQ1:BM1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:AO1"/>
-    <mergeCell ref="BH3:BI3"/>
-    <mergeCell ref="BL3:BM3"/>
-    <mergeCell ref="AR2:AW2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BE2:BI2"/>
-    <mergeCell ref="BJ2:BM2"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="K2:AN2"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="AK4:AN4"/>
+    <mergeCell ref="AF4:AI4"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AJ3:AN3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8465,26 +8424,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="32" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31" t="s">
+      <c r="H1" s="32"/>
+      <c r="I1" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="31"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9078,16 +9037,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.109375" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -9869,19 +9828,19 @@
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -9890,14 +9849,14 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -10062,16 +10021,16 @@
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="7" customWidth="1"/>
     <col min="4" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -10119,10 +10078,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
Remove space after Office-Conference
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwell\Documents\openstudio-standards\data\standards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4BA97A-1EF4-438A-AA1C-BEBF7F92DD88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07BBE1D-1104-41CB-A3FF-2F868EF7F814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="868" activeTab="5" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectInformation" sheetId="1" r:id="rId1"/>
@@ -352,9 +352,6 @@
     <t>Office-Corridor</t>
   </si>
   <si>
-    <t xml:space="preserve">Office-Conference </t>
-  </si>
-  <si>
     <t>Office-BreakRoom</t>
   </si>
   <si>
@@ -728,6 +725,9 @@
   </si>
   <si>
     <t>Ideal Air Loads with Ventilation</t>
+  </si>
+  <si>
+    <t>Office-Conference</t>
   </si>
 </sst>
 </file>
@@ -942,12 +942,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -955,6 +949,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1294,25 +1294,25 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.1328125" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1334,13 +1334,13 @@
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>24</v>
@@ -1348,7 +1348,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
@@ -1356,7 +1356,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1364,7 +1364,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1372,7 +1372,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1380,7 +1380,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -1388,55 +1388,55 @@
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -1459,14 +1459,14 @@
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.86328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.1328125" style="9"/>
-    <col min="8" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="1" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.109375" style="9"/>
+    <col min="8" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>150</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1544,7 +1544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1555,7 +1555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1566,7 +1566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1577,7 +1577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1588,7 +1588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1599,7 +1599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1610,7 +1610,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1621,7 +1621,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1632,7 +1632,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1643,7 +1643,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1654,7 +1654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1665,7 +1665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1676,7 +1676,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1687,7 +1687,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1698,7 +1698,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1709,7 +1709,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1720,7 +1720,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1731,7 +1731,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1742,7 +1742,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1753,7 +1753,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1764,7 +1764,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1775,7 +1775,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1786,7 +1786,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1797,7 +1797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1808,7 +1808,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1819,7 +1819,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1830,7 +1830,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1841,7 +1841,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1852,7 +1852,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1863,7 +1863,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1874,7 +1874,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1885,7 +1885,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1896,7 +1896,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1907,7 +1907,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1918,7 +1918,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1929,7 +1929,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1940,7 +1940,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1951,7 +1951,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1962,7 +1962,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1973,7 +1973,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1984,7 +1984,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1995,7 +1995,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2006,7 +2006,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2017,7 +2017,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2028,7 +2028,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2039,7 +2039,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2050,7 +2050,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2061,7 +2061,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2072,7 +2072,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -2083,7 +2083,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2094,7 +2094,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -2105,7 +2105,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2116,7 +2116,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -2127,7 +2127,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2138,7 +2138,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2149,7 +2149,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2160,7 +2160,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2171,7 +2171,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2182,7 +2182,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2193,7 +2193,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2204,7 +2204,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2215,7 +2215,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2226,7 +2226,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2237,7 +2237,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2248,7 +2248,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2259,7 +2259,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2270,7 +2270,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2281,7 +2281,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -2292,7 +2292,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2303,7 +2303,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2331,59 +2331,59 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.1328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="18.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="18.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="21" max="23" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="18.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="18.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="31" max="33" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="18.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="36" max="38" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="18.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.46484375" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14" style="9" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.86328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.86328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.86328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="6.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.46484375" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.86328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="7.46484375" style="9" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.86328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="6.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.46484375" style="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="16384" width="9.1328125" style="9"/>
+    <col min="62" max="62" width="8.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -2395,76 +2395,76 @@
         <v>28</v>
       </c>
       <c r="E1" s="26"/>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="29" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="31"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="29"/>
       <c r="AO1" s="26" t="s">
         <v>32</v>
       </c>
       <c r="AP1" s="26"/>
-      <c r="AQ1" s="28" t="s">
+      <c r="AQ1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="28"/>
-      <c r="BB1" s="28"/>
-      <c r="BC1" s="28"/>
-      <c r="BD1" s="28"/>
-      <c r="BE1" s="28"/>
-      <c r="BF1" s="28"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="28"/>
-      <c r="BI1" s="28"/>
-      <c r="BJ1" s="28"/>
-      <c r="BK1" s="28"/>
-      <c r="BL1" s="28"/>
-      <c r="BM1" s="28"/>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.45">
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>1</v>
@@ -2565,7 +2565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>200000</v>
       </c>
@@ -2596,48 +2596,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="29" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="29" t="s">
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="29" t="s">
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="29" t="s">
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="29" t="s">
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="30"/>
-      <c r="AL3" s="30"/>
-      <c r="AM3" s="30"/>
-      <c r="AN3" s="31"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="29"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2677,10 +2677,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="27" t="s">
+      <c r="BB3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="27"/>
+      <c r="BC3" s="31"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2690,25 +2690,25 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="27" t="s">
+      <c r="BG3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="27"/>
+      <c r="BH3" s="31"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="27" t="s">
+      <c r="BK3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="27"/>
+      <c r="BL3" s="31"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2734,57 +2734,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="29" t="s">
+      <c r="Q4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="31"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="29"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="31"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="29"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="29" t="s">
+      <c r="AA4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="31"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="29"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="29" t="s">
+      <c r="AF4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="31"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="29"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="29" t="s">
+      <c r="AK4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AN4" s="31"/>
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="29"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -2859,7 +2859,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="BM5" s="10"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -3159,7 +3159,7 @@
       </c>
       <c r="BM6" s="10"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="BM7" s="10"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -3381,7 +3381,7 @@
       </c>
       <c r="BM8" s="10"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="BM9" s="10"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -3581,7 +3581,7 @@
       <c r="BL10" s="3"/>
       <c r="BM10" s="3"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -3678,7 +3678,7 @@
       <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3">
@@ -3775,7 +3775,7 @@
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3872,7 +3872,7 @@
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3">
@@ -3969,7 +3969,7 @@
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -4066,7 +4066,7 @@
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -4163,7 +4163,7 @@
       <c r="BL16" s="3"/>
       <c r="BM16" s="3"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -4260,7 +4260,7 @@
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -4357,7 +4357,7 @@
       <c r="BL18" s="3"/>
       <c r="BM18" s="3"/>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -4454,7 +4454,7 @@
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -4527,7 +4527,7 @@
       <c r="BL20" s="3"/>
       <c r="BM20" s="3"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -4600,7 +4600,7 @@
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -4673,7 +4673,7 @@
       <c r="BL22" s="3"/>
       <c r="BM22" s="3"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -4746,7 +4746,7 @@
       <c r="BL23" s="3"/>
       <c r="BM23" s="3"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -4819,7 +4819,7 @@
       <c r="BL24" s="3"/>
       <c r="BM24" s="3"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3">
@@ -4892,7 +4892,7 @@
       <c r="BL25" s="3"/>
       <c r="BM25" s="3"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3">
@@ -4965,7 +4965,7 @@
       <c r="BL26" s="3"/>
       <c r="BM26" s="3"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
@@ -5038,7 +5038,7 @@
       <c r="BL27" s="3"/>
       <c r="BM27" s="3"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
@@ -5111,7 +5111,7 @@
       <c r="BL28" s="3"/>
       <c r="BM28" s="3"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
@@ -5184,7 +5184,7 @@
       <c r="BL29" s="3"/>
       <c r="BM29" s="3"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
@@ -5257,7 +5257,7 @@
       <c r="BL30" s="3"/>
       <c r="BM30" s="3"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
@@ -5330,7 +5330,7 @@
       <c r="BL31" s="3"/>
       <c r="BM31" s="3"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
@@ -5403,7 +5403,7 @@
       <c r="BL32" s="3"/>
       <c r="BM32" s="3"/>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3">
@@ -5476,7 +5476,7 @@
       <c r="BL33" s="3"/>
       <c r="BM33" s="3"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
@@ -5549,7 +5549,7 @@
       <c r="BL34" s="3"/>
       <c r="BM34" s="3"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
@@ -5622,7 +5622,7 @@
       <c r="BL35" s="3"/>
       <c r="BM35" s="3"/>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
@@ -5693,7 +5693,7 @@
       <c r="BL36" s="3"/>
       <c r="BM36" s="3"/>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3">
@@ -5764,7 +5764,7 @@
       <c r="BL37" s="3"/>
       <c r="BM37" s="3"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3">
@@ -5835,7 +5835,7 @@
       <c r="BL38" s="3"/>
       <c r="BM38" s="3"/>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3">
@@ -5906,7 +5906,7 @@
       <c r="BL39" s="3"/>
       <c r="BM39" s="3"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3">
@@ -5977,7 +5977,7 @@
       <c r="BL40" s="3"/>
       <c r="BM40" s="3"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3">
@@ -6048,7 +6048,7 @@
       <c r="BL41" s="3"/>
       <c r="BM41" s="3"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3">
@@ -6119,7 +6119,7 @@
       <c r="BL42" s="3"/>
       <c r="BM42" s="3"/>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3">
@@ -6190,7 +6190,7 @@
       <c r="BL43" s="3"/>
       <c r="BM43" s="3"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3">
@@ -6261,7 +6261,7 @@
       <c r="BL44" s="3"/>
       <c r="BM44" s="3"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3">
@@ -6332,7 +6332,7 @@
       <c r="BL45" s="3"/>
       <c r="BM45" s="3"/>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
@@ -6403,7 +6403,7 @@
       <c r="BL46" s="3"/>
       <c r="BM46" s="3"/>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3">
@@ -6474,7 +6474,7 @@
       <c r="BL47" s="3"/>
       <c r="BM47" s="3"/>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3">
@@ -6545,7 +6545,7 @@
       <c r="BL48" s="3"/>
       <c r="BM48" s="3"/>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3">
@@ -6616,7 +6616,7 @@
       <c r="BL49" s="3"/>
       <c r="BM49" s="3"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3">
@@ -6687,7 +6687,7 @@
       <c r="BL50" s="3"/>
       <c r="BM50" s="3"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3">
@@ -6758,7 +6758,7 @@
       <c r="BL51" s="3"/>
       <c r="BM51" s="3"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3">
@@ -6829,7 +6829,7 @@
       <c r="BL52" s="3"/>
       <c r="BM52" s="3"/>
     </row>
-    <row r="53" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6898,7 +6898,7 @@
       <c r="BL53" s="3"/>
       <c r="BM53" s="3"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6967,7 +6967,7 @@
       <c r="BL54" s="3"/>
       <c r="BM54" s="3"/>
     </row>
-    <row r="55" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -7036,7 +7036,7 @@
       <c r="BL55" s="3"/>
       <c r="BM55" s="3"/>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -7105,7 +7105,7 @@
       <c r="BL56" s="3"/>
       <c r="BM56" s="3"/>
     </row>
-    <row r="57" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -7174,7 +7174,7 @@
       <c r="BL57" s="3"/>
       <c r="BM57" s="3"/>
     </row>
-    <row r="58" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -7243,7 +7243,7 @@
       <c r="BL58" s="3"/>
       <c r="BM58" s="3"/>
     </row>
-    <row r="59" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -7312,7 +7312,7 @@
       <c r="BL59" s="3"/>
       <c r="BM59" s="3"/>
     </row>
-    <row r="60" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -7381,7 +7381,7 @@
       <c r="BL60" s="3"/>
       <c r="BM60" s="3"/>
     </row>
-    <row r="61" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -7450,7 +7450,7 @@
       <c r="BL61" s="3"/>
       <c r="BM61" s="3"/>
     </row>
-    <row r="62" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -7519,7 +7519,7 @@
       <c r="BL62" s="3"/>
       <c r="BM62" s="3"/>
     </row>
-    <row r="63" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -7588,7 +7588,7 @@
       <c r="BL63" s="3"/>
       <c r="BM63" s="3"/>
     </row>
-    <row r="64" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -7657,7 +7657,7 @@
       <c r="BL64" s="3"/>
       <c r="BM64" s="3"/>
     </row>
-    <row r="65" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -7726,7 +7726,7 @@
       <c r="BL65" s="3"/>
       <c r="BM65" s="3"/>
     </row>
-    <row r="66" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -7795,7 +7795,7 @@
       <c r="BL66" s="3"/>
       <c r="BM66" s="3"/>
     </row>
-    <row r="67" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -7864,7 +7864,7 @@
       <c r="BL67" s="3"/>
       <c r="BM67" s="3"/>
     </row>
-    <row r="68" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -7933,7 +7933,7 @@
       <c r="BL68" s="3"/>
       <c r="BM68" s="3"/>
     </row>
-    <row r="69" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -8002,7 +8002,7 @@
       <c r="BL69" s="3"/>
       <c r="BM69" s="3"/>
     </row>
-    <row r="70" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -8071,7 +8071,7 @@
       <c r="BL70" s="3"/>
       <c r="BM70" s="3"/>
     </row>
-    <row r="71" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -8140,7 +8140,7 @@
       <c r="BL71" s="3"/>
       <c r="BM71" s="3"/>
     </row>
-    <row r="72" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -8209,7 +8209,7 @@
       <c r="BL72" s="3"/>
       <c r="BM72" s="3"/>
     </row>
-    <row r="73" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -8278,7 +8278,7 @@
       <c r="BL73" s="3"/>
       <c r="BM73" s="3"/>
     </row>
-    <row r="74" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -8347,11 +8347,11 @@
       <c r="BL74" s="3"/>
       <c r="BM74" s="3"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -8365,6 +8365,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8381,23 +8398,6 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -8412,21 +8412,21 @@
       <selection activeCell="J23" sqref="A23:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.53125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" style="9" customWidth="1"/>
-    <col min="5" max="6" width="9.1328125" style="9"/>
-    <col min="7" max="7" width="6.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="9" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="9"/>
+    <col min="7" max="7" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="7"/>
+    <col min="11" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>80</v>
       </c>
@@ -8448,7 +8448,7 @@
       </c>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -8520,7 +8520,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>5</v>
@@ -8543,7 +8543,7 @@
       </c>
       <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>10</v>
@@ -8565,7 +8565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>15</v>
@@ -8587,7 +8587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>20</v>
@@ -8609,7 +8609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>25</v>
@@ -8631,7 +8631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>30</v>
@@ -8653,7 +8653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>35</v>
@@ -8675,7 +8675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>40</v>
@@ -8697,7 +8697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>45</v>
@@ -8719,7 +8719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>50</v>
@@ -8741,7 +8741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>55</v>
@@ -8764,7 +8764,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>60</v>
@@ -8791,7 +8791,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>65</v>
@@ -8813,7 +8813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>70</v>
@@ -8835,7 +8835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>75</v>
@@ -8857,7 +8857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>80</v>
@@ -8890,7 +8890,7 @@
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>85</v>
@@ -8910,7 +8910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>90</v>
@@ -8930,7 +8930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>95</v>
@@ -8950,7 +8950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8966,55 +8966,55 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" s="14"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="14"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="14"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="14"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="14"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="14"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="14"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="14"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="14"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="14"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="14"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="14"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="14"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="14"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="14"/>
     </row>
   </sheetData>
@@ -9034,24 +9034,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C609DAD-BC63-4626-ACCC-69F8C32CB7AB}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="7"/>
+    <col min="2" max="2" width="34.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -9059,7 +9059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -9067,748 +9067,748 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="18" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="16"/>
       <c r="B103" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="16"/>
       <c r="B104" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
       <c r="B105" s="18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="16"/>
       <c r="B106" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="16"/>
       <c r="B107" s="18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="16"/>
       <c r="B108" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
       <c r="B109" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="16"/>
       <c r="B110" s="18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="16"/>
       <c r="B111" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="16"/>
       <c r="B113" s="18" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="16"/>
       <c r="B114" s="18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="16"/>
       <c r="B115" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="16"/>
       <c r="B116" s="18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="16"/>
       <c r="B117" s="18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="16"/>
       <c r="B118" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="16"/>
       <c r="B119" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="16"/>
       <c r="B120" s="18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="16"/>
       <c r="B121" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="16"/>
       <c r="B123" s="18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="16"/>
       <c r="B124" s="18" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="16"/>
       <c r="B125" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="16"/>
       <c r="B126" s="18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="16"/>
       <c r="B127" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -9824,28 +9824,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84235012-AF5A-4BF0-8557-E62F3FAF9D19}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="7"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -9853,15 +9853,15 @@
         <v>2</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D2" s="35"/>
       <c r="E2" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F2" s="35"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>98</v>
       </c>
@@ -9881,7 +9881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
         <v>92</v>
@@ -9899,7 +9899,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
         <v>93</v>
@@ -9913,7 +9913,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
         <v>94</v>
@@ -9927,7 +9927,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
         <v>95</v>
@@ -9941,7 +9941,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
         <v>96</v>
@@ -9955,7 +9955,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
         <v>97</v>
@@ -9969,7 +9969,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="15" t="s">
         <v>98</v>
@@ -9979,7 +9979,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
         <v>99</v>
@@ -9989,7 +9989,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
         <v>100</v>
@@ -9999,10 +9999,10 @@
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -10028,21 +10028,21 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.1328125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="9" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="7"/>
+    <col min="4" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -10050,7 +10050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>89</v>
@@ -10080,20 +10080,20 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" style="9"/>
-    <col min="3" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="1" width="11.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="9"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -10101,7 +10101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>50</v>
       </c>
@@ -10109,115 +10109,115 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
Excel autocorrects cafe->café when editing CSV files, this commit changes that back
Suggest that developers delete this auto correction in Excel

https://www.ablebits.com/office-addins-blog/2018/08/22/customize-stop-autocorrect-excel/
</commit_message>
<xml_diff>
--- a/data/standards/InputJSONData.xlsx
+++ b/data/standards/InputJSONData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pw-openstudio-standards\data\standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07BBE1D-1104-41CB-A3FF-2F868EF7F814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB54548-290B-4892-932C-14C45D77557D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="4" xr2:uid="{17BA9D28-F428-4320-951B-A5253BE2BB9F}"/>
   </bookViews>
@@ -451,9 +451,6 @@
     <t>LrgHotel-Basement</t>
   </si>
   <si>
-    <t>LrgHotel-Café</t>
-  </si>
-  <si>
     <t>LrgHotel-Corridor</t>
   </si>
   <si>
@@ -490,9 +487,6 @@
     <t>Outpatient-BioHazard</t>
   </si>
   <si>
-    <t>Outpatient-Café</t>
-  </si>
-  <si>
     <t>Outpatient-Conference</t>
   </si>
   <si>
@@ -728,6 +722,12 @@
   </si>
   <si>
     <t>Office-Conference</t>
+  </si>
+  <si>
+    <t>LrgHotel-Cafe</t>
+  </si>
+  <si>
+    <t>Outpatient-Cafe</t>
   </si>
 </sst>
 </file>
@@ -942,6 +942,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,12 +955,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D1" s="26"/>
     </row>
@@ -1334,10 +1334,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2395,74 +2395,74 @@
         <v>28</v>
       </c>
       <c r="E1" s="26"/>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="31"/>
       <c r="AO1" s="26" t="s">
         <v>32</v>
       </c>
       <c r="AP1" s="26"/>
-      <c r="AQ1" s="30" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+      <c r="AX1" s="28"/>
+      <c r="AY1" s="28"/>
+      <c r="AZ1" s="28"/>
+      <c r="BA1" s="28"/>
+      <c r="BB1" s="28"/>
+      <c r="BC1" s="28"/>
+      <c r="BD1" s="28"/>
+      <c r="BE1" s="28"/>
+      <c r="BF1" s="28"/>
+      <c r="BG1" s="28"/>
+      <c r="BH1" s="28"/>
+      <c r="BI1" s="28"/>
+      <c r="BJ1" s="28"/>
+      <c r="BK1" s="28"/>
+      <c r="BL1" s="28"/>
+      <c r="BM1" s="28"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>1</v>
@@ -2596,48 +2596,48 @@
       <c r="J3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="27" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="27" t="s">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="27" t="s">
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="27" t="s">
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
-      <c r="AJ3" s="27" t="s">
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="29"/>
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="30"/>
+      <c r="AM3" s="30"/>
+      <c r="AN3" s="31"/>
       <c r="AO3" s="3">
         <v>0</v>
       </c>
@@ -2677,10 +2677,10 @@
       <c r="BA3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BB3" s="31" t="s">
+      <c r="BB3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BC3" s="31"/>
+      <c r="BC3" s="27"/>
       <c r="BD3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2690,20 +2690,20 @@
       <c r="BF3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="31" t="s">
+      <c r="BG3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BH3" s="31"/>
+      <c r="BH3" s="27"/>
       <c r="BI3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BK3" s="31" t="s">
+      <c r="BK3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BL3" s="31"/>
+      <c r="BL3" s="27"/>
       <c r="BM3" s="10" t="s">
         <v>1</v>
       </c>
@@ -2734,57 +2734,57 @@
       <c r="K4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="29"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="31"/>
       <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="29"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
       <c r="U4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="27" t="s">
+      <c r="V4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="29"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="31"/>
       <c r="Z4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="27" t="s">
+      <c r="AA4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="29"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="31"/>
       <c r="AE4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="27" t="s">
+      <c r="AF4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="29"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="31"/>
       <c r="AJ4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AK4" s="27" t="s">
+      <c r="AK4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="28"/>
-      <c r="AM4" s="28"/>
-      <c r="AN4" s="29"/>
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="31"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3">
         <v>5</v>
@@ -8365,23 +8365,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BH2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="BB3:BC3"/>
-    <mergeCell ref="AQ1:BM1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:AN1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N5:O5"/>
@@ -8398,6 +8381,23 @@
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:BM1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:AN1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -9034,8 +9034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C609DAD-BC63-4626-ACCC-69F8C32CB7AB}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9046,10 +9046,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -9094,7 +9094,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9304,511 +9304,511 @@
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="18" t="s">
-        <v>139</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="18" t="s">
-        <v>152</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="16"/>
       <c r="B103" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="16"/>
       <c r="B104" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
       <c r="B105" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="16"/>
       <c r="B106" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="16"/>
       <c r="B107" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="16"/>
       <c r="B108" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
       <c r="B109" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="16"/>
       <c r="B110" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="16"/>
       <c r="B111" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="16"/>
       <c r="B113" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="16"/>
       <c r="B114" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="16"/>
       <c r="B115" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="16"/>
       <c r="B116" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="16"/>
       <c r="B117" s="18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="16"/>
       <c r="B118" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="16"/>
       <c r="B119" s="18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="16"/>
       <c r="B120" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="16"/>
       <c r="B121" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="16"/>
       <c r="B123" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="16"/>
       <c r="B124" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="16"/>
       <c r="B125" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="16"/>
       <c r="B126" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="16"/>
       <c r="B127" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -9836,14 +9836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -9853,11 +9853,11 @@
         <v>2</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D2" s="35"/>
       <c r="E2" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F2" s="35"/>
     </row>
@@ -10002,7 +10002,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>

</xml_diff>